<commit_message>
Spring Data JPA, Angular JS, Maven, Junit
Spring Data JPA, Angular JS, Maven, Junit
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="595">
   <si>
     <t>Main Topic</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Spring AOP</t>
-  </si>
-  <si>
-    <t>Spring JDBS/DAO</t>
   </si>
   <si>
     <t>Java based configurations</t>
@@ -4316,6 +4313,102 @@
   </si>
   <si>
     <t>Spring ORM/JPA</t>
+  </si>
+  <si>
+    <t>Spring Batch</t>
+  </si>
+  <si>
+    <t>Spring Data Mango</t>
+  </si>
+  <si>
+    <t>Github link</t>
+  </si>
+  <si>
+    <t>https://github.com/avinashbabudonthu/SpringDataPractice.git</t>
+  </si>
+  <si>
+    <t>Create mavenized project using</t>
+  </si>
+  <si>
+    <t>maven archetype:generate ------</t>
+  </si>
+  <si>
+    <t>Add spring-data-jpa dependency to pom.xml</t>
+  </si>
+  <si>
+    <t>&lt;dependency&gt;
+   &lt;groupId&gt;org.springframework.data&lt;/groupId&gt;
+   &lt;artifactId&gt;spring-data-jpa&lt;/artifactId&gt;
+   &lt;version&gt;1.10.5.RELEASE&lt;/version&gt;
+  &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>If we are using xml file, we need to add this entry in spring xml configuration file</t>
+  </si>
+  <si>
+    <t>&lt;jpa:repositories base-package="spring.data.jpa.repositories"/&gt;</t>
+  </si>
+  <si>
+    <t>Using this spring will scan the package for repository classes</t>
+  </si>
+  <si>
+    <t>If we are using Spring Boot (or) Java Configurations we need to use this annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @EnableJpaRepositories</t>
+  </si>
+  <si>
+    <t>org.springframework.data.jpa.repository.JpaRepository</t>
+  </si>
+  <si>
+    <t>All Spring data repository interfaces has to extend this interface</t>
+  </si>
+  <si>
+    <t>JpaRepository class hierarchy</t>
+  </si>
+  <si>
+    <t>Refer images\3_Spring\3_Spring_Data\1_Jpa_Repository_call_hierarchy.jpg</t>
+  </si>
+  <si>
+    <t>query parser will match these keywords</t>
+  </si>
+  <si>
+    <t>1. find..By
+2. query..By
+3. read..By
+4. count..By
+5. get..By</t>
+  </si>
+  <si>
+    <t>Spring Data JPA Auditing annotation</t>
+  </si>
+  <si>
+    <t>1. @CreatedBy
+2. @CreatedDate
+3. @LastModifiedBy
+3. @LastModifiedDate</t>
+  </si>
+  <si>
+    <t>Above annotation have to be declared in entity class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Entity
+public class Model{
+@CreatedBy private User user;
+@CreatedDate private DateTime createDate;
+}</t>
+  </si>
+  <si>
+    <t>Auditing implementation in Spring Data JPA</t>
+  </si>
+  <si>
+    <t>Refer images\3_Spring\3_Spring_Data\2_Auding_implementation.jpg</t>
+  </si>
+  <si>
+    <t>Locking implementation in Spring Data JPA</t>
+  </si>
+  <si>
+    <t>Refer images\3_Spring\3_Spring_Data\3_Locking_implementation.jpg</t>
   </si>
 </sst>
 </file>
@@ -4529,7 +4622,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4670,6 +4763,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5045,11 +5150,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5064,30 +5169,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="14" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="1"/>
@@ -5101,7 +5206,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="20"/>
@@ -5129,61 +5234,68 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B15" s="15"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>347</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="22"/>
+      <c r="A18" s="22" t="s">
+        <v>568</v>
+      </c>
       <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="22" t="s">
+        <v>569</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5225,10 +5337,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5257,10 +5369,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5289,114 +5401,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="60"/>
+      <c r="A4" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="120">
+      <c r="A6" s="71"/>
+      <c r="B6" s="7" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="67"/>
-      <c r="B6" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60">
       <c r="A8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90">
       <c r="A9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="90">
       <c r="A11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="30">
+      <c r="A12" s="77" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="73" t="s">
+      <c r="B12" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="45">
+      <c r="A13" s="77"/>
+      <c r="B13" s="7" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="73"/>
-      <c r="B13" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="77" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="73" t="s">
+      <c r="B15" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="285">
+      <c r="A16" s="77"/>
+      <c r="B16" s="7" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="73"/>
-      <c r="B16" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -5419,8 +5531,8 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5431,454 +5543,454 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="59" t="s">
-        <v>423</v>
-      </c>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>389</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="59" t="s">
-        <v>308</v>
-      </c>
-      <c r="B6" s="60"/>
+      <c r="A6" s="63" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" s="64"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60">
       <c r="A8" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>364</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>366</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>368</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120">
       <c r="A11" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>371</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60">
       <c r="A13" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>377</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>379</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>381</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45">
       <c r="A16" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>384</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
       <c r="A18" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>387</v>
       </c>
-      <c r="B18" s="32" t="s">
-        <v>388</v>
-      </c>
     </row>
     <row r="19" spans="1:2" ht="45">
-      <c r="A19" s="70" t="s">
-        <v>393</v>
+      <c r="A19" s="74" t="s">
+        <v>392</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="70"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="32" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45">
       <c r="A21" s="32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
       <c r="A22" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="B23" s="32" t="s">
         <v>395</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>398</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="75">
       <c r="A25" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30">
       <c r="A26" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="B26" s="27" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="75" t="s">
+        <v>403</v>
+      </c>
+      <c r="B27" s="32" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="71" t="s">
+    <row r="28" spans="1:2" ht="120">
+      <c r="A28" s="75"/>
+      <c r="B28" s="32" t="s">
         <v>404</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="120">
-      <c r="A28" s="71"/>
-      <c r="B28" s="32" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30">
       <c r="A29" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B29" s="32" t="s">
         <v>406</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="B30" s="32" t="s">
         <v>408</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
       <c r="A31" s="32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
       <c r="A32" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="105">
       <c r="A33" s="57" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90">
       <c r="A34" s="33" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="225">
       <c r="A35" s="35" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30">
       <c r="A36" s="35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="22" customFormat="1">
       <c r="A39" s="48" t="s">
+        <v>508</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>509</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="105">
       <c r="A40" s="48" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="45">
-      <c r="A41" s="71" t="s">
-        <v>520</v>
+      <c r="A41" s="75" t="s">
+        <v>519</v>
       </c>
       <c r="B41" s="51" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="210">
+      <c r="A42" s="75"/>
+      <c r="B42" s="51" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="210">
-      <c r="A42" s="71"/>
-      <c r="B42" s="51" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
       <c r="A43" s="52" t="s">
+        <v>520</v>
+      </c>
+      <c r="B43" s="52" t="s">
         <v>521</v>
-      </c>
-      <c r="B43" s="52" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="52" t="s">
+        <v>522</v>
+      </c>
+      <c r="B44" s="52" t="s">
         <v>523</v>
       </c>
-      <c r="B44" s="52" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="30">
+      <c r="A45" s="79" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="75" t="s">
+      <c r="B45" s="52" t="s">
         <v>525</v>
       </c>
-      <c r="B45" s="52" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="120">
+      <c r="A46" s="79"/>
+      <c r="B46" s="52" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="79"/>
+      <c r="B47" s="27" t="s">
         <v>526</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="120">
-      <c r="A46" s="75"/>
-      <c r="B46" s="52" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="75"/>
-      <c r="B47" s="27" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60">
       <c r="A48" s="53" t="s">
+        <v>528</v>
+      </c>
+      <c r="B48" s="56" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="45" customHeight="1">
+      <c r="A49" s="79" t="s">
         <v>529</v>
       </c>
-      <c r="B48" s="56" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="45" customHeight="1">
-      <c r="A49" s="75" t="s">
+      <c r="B49" s="53" t="s">
         <v>530</v>
       </c>
-      <c r="B49" s="53" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="30">
+      <c r="A50" s="79"/>
+      <c r="B50" s="53" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="75"/>
-      <c r="B50" s="53" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
       <c r="A51" s="53" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="22" customFormat="1" ht="30">
       <c r="A52" s="53" t="s">
+        <v>537</v>
+      </c>
+      <c r="B52" s="53" t="s">
         <v>538</v>
-      </c>
-      <c r="B52" s="53" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="45">
       <c r="A53" s="53" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="53" t="s">
+        <v>535</v>
+      </c>
+      <c r="B54" s="53" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="79" t="s">
         <v>536</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B55" s="53" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="75" t="s">
-        <v>537</v>
-      </c>
-      <c r="B55" s="53" t="s">
+    <row r="56" spans="1:2" ht="60">
+      <c r="A56" s="79"/>
+      <c r="B56" s="53" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="60">
-      <c r="A56" s="75"/>
-      <c r="B56" s="53" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="53" t="s">
+        <v>543</v>
+      </c>
+      <c r="B57" s="53" t="s">
         <v>544</v>
       </c>
-      <c r="B57" s="53" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="45">
+      <c r="A58" s="78" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="74" t="s">
+      <c r="B58" s="55" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="78"/>
+      <c r="B59" s="54" t="s">
         <v>546</v>
-      </c>
-      <c r="B58" s="55" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="74"/>
-      <c r="B59" s="54" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
       <c r="A60" s="55" t="s">
+        <v>548</v>
+      </c>
+      <c r="B60" s="55" t="s">
         <v>549</v>
-      </c>
-      <c r="B60" s="55" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="55" t="s">
+        <v>550</v>
+      </c>
+      <c r="B61" s="55" t="s">
         <v>551</v>
-      </c>
-      <c r="B61" s="55" t="s">
-        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -5924,17 +6036,17 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="59" t="s">
-        <v>317</v>
-      </c>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="23" t="s">
@@ -5945,139 +6057,139 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="59" t="s">
-        <v>318</v>
-      </c>
-      <c r="B6" s="60"/>
+      <c r="A6" s="63" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="64"/>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>320</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75">
       <c r="A10" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>325</v>
-      </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="B11" s="29" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="30">
+      <c r="A12" s="79"/>
+      <c r="B12" s="29" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="75"/>
-      <c r="B12" s="29" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="75">
       <c r="A13" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="70" t="s">
-        <v>340</v>
+      <c r="A14" s="74" t="s">
+        <v>339</v>
       </c>
       <c r="B14" s="29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="180">
+      <c r="A15" s="74"/>
+      <c r="B15" s="29" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="70"/>
-      <c r="B15" s="29" t="s">
-        <v>353</v>
-      </c>
-    </row>
     <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="70"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="22" customFormat="1" ht="30">
       <c r="A17" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90">
       <c r="A18" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="22" customFormat="1" ht="120">
       <c r="A19" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>357</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
       <c r="A20" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>342</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>349</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
       <c r="A23" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>360</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -6100,55 +6212,159 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" style="59" customWidth="1"/>
     <col min="2" max="2" width="135.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="59" t="s">
-        <v>423</v>
-      </c>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="64"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="59" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="59" t="s">
-        <v>318</v>
-      </c>
-      <c r="B7" s="60"/>
+      <c r="A7" s="63" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="64"/>
     </row>
     <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="59" t="s">
+        <v>564</v>
+      </c>
+      <c r="B8" s="58" t="s">
         <v>565</v>
       </c>
-      <c r="B8" s="58" t="s">
-        <v>566</v>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="59" t="s">
+        <v>572</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="75">
+      <c r="A10" s="59" t="s">
+        <v>574</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1">
+      <c r="A11" s="78" t="s">
+        <v>576</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="78"/>
+      <c r="B12" s="22" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
+      <c r="A13" s="59" t="s">
+        <v>579</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="60" t="s">
+        <v>582</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="60" t="s">
+        <v>583</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="75">
+      <c r="A16" s="61" t="s">
+        <v>585</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="60">
+      <c r="A17" s="62" t="s">
+        <v>587</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="75">
+      <c r="A18" s="62" t="s">
+        <v>589</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="62" t="s">
+        <v>591</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="62" t="s">
+        <v>593</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A15" display="Topics"/>
     <hyperlink ref="B1" location="Data!A2" display="Up"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6172,220 +6388,220 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C1" s="47" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="22" customFormat="1">
-      <c r="A2" s="59" t="s">
-        <v>499</v>
-      </c>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="22" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="22" customFormat="1"/>
     <row r="5" spans="1:3">
-      <c r="A5" s="59" t="s">
-        <v>307</v>
-      </c>
-      <c r="B5" s="60"/>
+      <c r="A5" s="63" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="64"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>373</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>374</v>
-      </c>
       <c r="C6" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="39" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="62"/>
+      <c r="A9" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="66"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>480</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>481</v>
-      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="60"/>
+      <c r="B12" s="64"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>227</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>444</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>466</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>469</v>
-      </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="59" t="s">
-        <v>291</v>
-      </c>
-      <c r="B21" s="60"/>
+      <c r="A21" s="63" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="64"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>375</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>303</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>304</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="59" t="s">
-        <v>564</v>
-      </c>
-      <c r="B28" s="60"/>
+      <c r="A28" s="63" t="s">
+        <v>563</v>
+      </c>
+      <c r="B28" s="64"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="60"/>
+      <c r="B33" s="64"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -6435,606 +6651,606 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="61" t="s">
-        <v>423</v>
-      </c>
-      <c r="B2" s="62"/>
+      <c r="A2" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="66"/>
     </row>
     <row r="3" spans="1:2" s="22" customFormat="1"/>
     <row r="4" spans="1:2" s="22" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="62"/>
+      <c r="A5" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="66"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="73"/>
+      <c r="B7" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="69"/>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135">
       <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="345">
       <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="45">
+      <c r="A10" s="70" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="45">
-      <c r="A10" s="66" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="71"/>
+      <c r="B11" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30">
-      <c r="A11" s="67"/>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60">
       <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
       <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="60">
       <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45">
       <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120">
       <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="60">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="60">
       <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45">
       <c r="A21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
       <c r="A22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60">
       <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="75">
       <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="105">
       <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="45">
       <c r="A26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
       <c r="A27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="75">
       <c r="A30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
       <c r="A31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="105">
       <c r="A32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60">
       <c r="A33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
       <c r="A34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120">
       <c r="A35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="45">
       <c r="A36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="165">
       <c r="A37" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="255">
       <c r="A38" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
       <c r="A40" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="60">
       <c r="A41" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30">
       <c r="A42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30">
       <c r="A43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45">
       <c r="A44" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="45">
       <c r="A45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="7" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="45">
+      <c r="A46" s="71" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="45">
-      <c r="A46" s="67" t="s">
+      <c r="B46" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="7" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="45">
+      <c r="A47" s="71"/>
+      <c r="B47" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="45">
-      <c r="A47" s="67"/>
-      <c r="B47" s="7" t="s">
+    <row r="48" spans="1:2" ht="60">
+      <c r="A48" s="71"/>
+      <c r="B48" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="60">
-      <c r="A48" s="67"/>
-      <c r="B48" s="7" t="s">
+    <row r="49" spans="1:2" ht="45">
+      <c r="A49" s="71" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="45">
-      <c r="A49" s="67" t="s">
+      <c r="B49" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="7" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="30">
+      <c r="A50" s="71"/>
+      <c r="B50" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="67"/>
-      <c r="B50" s="7" t="s">
+    <row r="51" spans="1:2" ht="90">
+      <c r="A51" s="71"/>
+      <c r="B51" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="90">
-      <c r="A51" s="67"/>
-      <c r="B51" s="7" t="s">
+    <row r="52" spans="1:2" ht="75">
+      <c r="A52" s="71" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="75">
-      <c r="A52" s="67" t="s">
+      <c r="B52" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="53" spans="1:2" ht="45">
-      <c r="A53" s="67"/>
+      <c r="A53" s="71"/>
       <c r="B53" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30">
       <c r="A57" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
       <c r="A58" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="60">
       <c r="A59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B59" s="7" t="s">
+    </row>
+    <row r="60" spans="1:2" ht="30">
+      <c r="A60" s="69" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="30">
-      <c r="A60" s="65" t="s">
+      <c r="B60" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="7" t="s">
+    </row>
+    <row r="61" spans="1:2" ht="240">
+      <c r="A61" s="69"/>
+      <c r="B61" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="240">
-      <c r="A61" s="65"/>
-      <c r="B61" s="7" t="s">
+    <row r="62" spans="1:2" ht="180">
+      <c r="A62" s="69"/>
+      <c r="B62" s="7" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="180">
-      <c r="A62" s="65"/>
-      <c r="B62" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30">
       <c r="A63" s="49" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135">
       <c r="A64" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150">
       <c r="A65" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="B65" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="60">
       <c r="A66" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="B66" s="35" t="s">
         <v>420</v>
-      </c>
-      <c r="B66" s="35" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30">
       <c r="A67" s="37" t="s">
+        <v>472</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="105">
+      <c r="A68" s="68" t="s">
+        <v>476</v>
+      </c>
+      <c r="B68" s="38" t="s">
         <v>473</v>
       </c>
-      <c r="B67" s="38" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="105">
-      <c r="A68" s="64" t="s">
+    </row>
+    <row r="69" spans="1:2" ht="120">
+      <c r="A69" s="68"/>
+      <c r="B69" s="38" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="75">
+      <c r="A70" s="68"/>
+      <c r="B70" s="38" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="60">
+      <c r="A71" s="68" t="s">
         <v>477</v>
       </c>
-      <c r="B68" s="38" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="120">
-      <c r="A69" s="64"/>
-      <c r="B69" s="38" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="75">
-      <c r="A70" s="64"/>
-      <c r="B70" s="38" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="60">
-      <c r="A71" s="64" t="s">
-        <v>478</v>
-      </c>
       <c r="B71" s="46" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60">
-      <c r="A72" s="64"/>
+      <c r="A72" s="68"/>
       <c r="B72" s="46" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30">
       <c r="A73" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="B73" s="41" t="s">
         <v>482</v>
-      </c>
-      <c r="B73" s="41" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60">
       <c r="A74" s="40" t="s">
+        <v>483</v>
+      </c>
+      <c r="B74" s="41" t="s">
         <v>484</v>
-      </c>
-      <c r="B74" s="41" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="45">
       <c r="A75" s="40" t="s">
+        <v>485</v>
+      </c>
+      <c r="B75" s="41" t="s">
         <v>486</v>
-      </c>
-      <c r="B75" s="41" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30">
       <c r="A76" s="40" t="s">
+        <v>487</v>
+      </c>
+      <c r="B76" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="B76" s="41" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75">
       <c r="A77" s="44" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="B78" s="43" t="s">
         <v>492</v>
-      </c>
-      <c r="B78" s="43" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="45">
       <c r="A79" s="42" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="63" t="s">
+      <c r="A80" s="67" t="s">
+        <v>503</v>
+      </c>
+      <c r="B80" s="46" t="s">
         <v>504</v>
       </c>
-      <c r="B80" s="46" t="s">
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="67"/>
+      <c r="B81" s="46" t="s">
         <v>505</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="63"/>
-      <c r="B81" s="46" t="s">
-        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -7078,208 +7294,208 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="60"/>
+      <c r="A4" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="A11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45">
       <c r="A12" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
       <c r="A21" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
       <c r="A25" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -7298,7 +7514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -7311,24 +7527,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="B3" s="60"/>
+      <c r="A3" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -7360,184 +7576,184 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="1:2" ht="90">
       <c r="A4" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135">
       <c r="A6" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30">
       <c r="A17" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
       <c r="A20" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
       <c r="A21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30">
       <c r="A24" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -7570,17 +7786,17 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:2" s="22" customFormat="1">
-      <c r="A2" s="59" t="s">
-        <v>423</v>
-      </c>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2" s="22" customFormat="1">
       <c r="A3" s="8"/>
@@ -7591,268 +7807,263 @@
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="59" t="s">
-        <v>318</v>
-      </c>
-      <c r="B5" s="60"/>
+      <c r="A5" s="63" t="s">
+        <v>317</v>
+      </c>
+      <c r="B5" s="64"/>
     </row>
     <row r="6" spans="1:2" ht="75">
       <c r="A6" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>236</v>
-      </c>
     </row>
     <row r="7" spans="1:2" ht="120">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="71" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>311</v>
       </c>
-      <c r="B7" s="12" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="240">
+      <c r="A8" s="71"/>
+      <c r="B8" s="12" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="240">
-      <c r="A8" s="67"/>
-      <c r="B8" s="12" t="s">
-        <v>313</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" ht="60">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="B9" s="12" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="255">
+      <c r="A10" s="68"/>
+      <c r="B10" s="12" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="255">
-      <c r="A10" s="64"/>
-      <c r="B10" s="12" t="s">
+    <row r="11" spans="1:2" ht="150">
+      <c r="A11" s="68"/>
+      <c r="B11" s="12" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="150">
-      <c r="A11" s="64"/>
-      <c r="B11" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
     <row r="12" spans="1:2" ht="150">
-      <c r="A12" s="70" t="s">
-        <v>446</v>
+      <c r="A12" s="74" t="s">
+        <v>445</v>
       </c>
       <c r="B12" s="36" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="22" customFormat="1" ht="105">
+      <c r="A13" s="74"/>
+      <c r="B13" s="36" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="22" customFormat="1" ht="105">
-      <c r="A13" s="70"/>
-      <c r="B13" s="36" t="s">
-        <v>471</v>
-      </c>
-    </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="74" t="s">
+        <v>423</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="B14" s="36" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="60">
+      <c r="A15" s="74"/>
+      <c r="B15" s="36" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60">
-      <c r="A15" s="70"/>
-      <c r="B15" s="36" t="s">
+    <row r="16" spans="1:2" ht="45">
+      <c r="A16" s="74"/>
+      <c r="B16" s="36" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45">
-      <c r="A16" s="70"/>
-      <c r="B16" s="36" t="s">
+    <row r="17" spans="1:2" ht="30">
+      <c r="A17" s="74" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="70" t="s">
+      <c r="B17" s="36" t="s">
         <v>428</v>
       </c>
-      <c r="B17" s="36" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="135">
+      <c r="A18" s="74"/>
+      <c r="B18" s="36" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="135">
-      <c r="A18" s="70"/>
-      <c r="B18" s="36" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="74"/>
+      <c r="B19" s="36" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="70"/>
-      <c r="B19" s="36" t="s">
+    <row r="20" spans="1:2" ht="45">
+      <c r="A20" s="74"/>
+      <c r="B20" s="36" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="70"/>
-      <c r="B20" s="36" t="s">
+    <row r="21" spans="1:2" ht="30">
+      <c r="A21" s="74"/>
+      <c r="B21" s="36" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="70"/>
-      <c r="B21" s="36" t="s">
+    <row r="22" spans="1:2" ht="45">
+      <c r="A22" s="75" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="71" t="s">
+      <c r="B22" s="36" t="s">
         <v>434</v>
       </c>
-      <c r="B22" s="36" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="45">
+      <c r="A23" s="75"/>
+      <c r="B23" s="36" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="45">
-      <c r="A23" s="71"/>
-      <c r="B23" s="36" t="s">
+    <row r="24" spans="1:2" ht="30">
+      <c r="A24" s="75"/>
+      <c r="B24" s="36" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30">
-      <c r="A24" s="71"/>
-      <c r="B24" s="36" t="s">
+    <row r="25" spans="1:2" ht="45">
+      <c r="A25" s="75"/>
+      <c r="B25" s="36" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="71"/>
-      <c r="B25" s="36" t="s">
+    <row r="26" spans="1:2" ht="45">
+      <c r="A26" s="75"/>
+      <c r="B26" s="36" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="45">
-      <c r="A26" s="71"/>
-      <c r="B26" s="36" t="s">
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="74" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="70" t="s">
+      <c r="B27" s="36" t="s">
         <v>440</v>
       </c>
-      <c r="B27" s="36" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="165">
+      <c r="A28" s="74"/>
+      <c r="B28" s="36" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="165">
-      <c r="A28" s="70"/>
-      <c r="B28" s="36" t="s">
+    <row r="29" spans="1:2" ht="30">
+      <c r="A29" s="74"/>
+      <c r="B29" s="36" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="70"/>
-      <c r="B29" s="36" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30">
       <c r="A30" s="50" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="60">
       <c r="A31" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="B31" s="36" t="s">
         <v>448</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
       <c r="A32" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="B32" s="36" t="s">
         <v>450</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="75">
       <c r="A33" s="36" t="s">
+        <v>451</v>
+      </c>
+      <c r="B33" s="36" t="s">
         <v>452</v>
       </c>
-      <c r="B33" s="36" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="30">
+      <c r="A34" s="74" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="70" t="s">
+      <c r="B34" s="36" t="s">
         <v>454</v>
       </c>
-      <c r="B34" s="36" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="75">
+      <c r="A35" s="74"/>
+      <c r="B35" s="36" t="s">
         <v>455</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="75">
-      <c r="A35" s="70"/>
-      <c r="B35" s="36" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120">
       <c r="A36" s="36" t="s">
+        <v>456</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>457</v>
       </c>
-      <c r="B36" s="36" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="74" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="70" t="s">
+      <c r="B37" s="36" t="s">
         <v>459</v>
       </c>
-      <c r="B37" s="36" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="30">
+      <c r="A38" s="74"/>
+      <c r="B38" s="36" t="s">
         <v>460</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30">
-      <c r="A38" s="70"/>
-      <c r="B38" s="36" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135">
       <c r="A39" s="36" t="s">
+        <v>461</v>
+      </c>
+      <c r="B39" s="36" t="s">
         <v>462</v>
       </c>
-      <c r="B39" s="36" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="30">
+      <c r="A40" s="74" t="s">
+        <v>458</v>
+      </c>
+      <c r="B40" s="36" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="70" t="s">
-        <v>459</v>
-      </c>
-      <c r="B40" s="36" t="s">
+    <row r="41" spans="1:2" ht="60">
+      <c r="A41" s="74"/>
+      <c r="B41" s="36" t="s">
         <v>464</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="60">
-      <c r="A41" s="70"/>
-      <c r="B41" s="36" t="s">
-        <v>465</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A37:A38"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
@@ -7860,6 +8071,11 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -7887,248 +8103,248 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="1:2" ht="60">
       <c r="A4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
       <c r="A5" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60">
       <c r="A9" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="71" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="67" t="s">
+      <c r="B10" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="45">
+      <c r="A11" s="71"/>
+      <c r="B11" s="7" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="67"/>
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="1:2" ht="60">
+      <c r="A12" s="71"/>
+      <c r="B12" s="7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="67"/>
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="76" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="72" t="s">
+      <c r="B13" s="76"/>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="71" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="72"/>
-    </row>
-    <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="67" t="s">
+      <c r="B14" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="71"/>
+      <c r="B15" s="7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="67"/>
-      <c r="B15" s="7" t="s">
+    <row r="16" spans="1:2" ht="60">
+      <c r="A16" s="71"/>
+      <c r="B16" s="7" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="60">
-      <c r="A16" s="67"/>
-      <c r="B16" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="71" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="67" t="s">
+      <c r="B20" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="B20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="75">
+      <c r="A21" s="71"/>
+      <c r="B21" s="7" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="67"/>
-      <c r="B21" s="7" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="105">
       <c r="A25" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>275</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B30" s="7" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="30">
+      <c r="A31" s="71" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="67" t="s">
+      <c r="B31" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B31" s="7" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="30">
+      <c r="A32" s="71"/>
+      <c r="B32" s="7" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="67"/>
-      <c r="B32" s="7" t="s">
+    <row r="33" spans="1:2" ht="45">
+      <c r="A33" s="71"/>
+      <c r="B33" s="7" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="67"/>
-      <c r="B33" s="7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30">
       <c r="A34" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -8165,10 +8381,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="22" customFormat="1"/>
@@ -8176,41 +8392,41 @@
       <c r="B8" s="15"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="59" t="s">
-        <v>298</v>
-      </c>
-      <c r="B10" s="60"/>
+      <c r="A10" s="63" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="64"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11" t="s">
         <v>294</v>
       </c>
-      <c r="B11" t="s">
-        <v>295</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="59" t="s">
-        <v>292</v>
-      </c>
-      <c r="B15" s="60"/>
+      <c r="A15" s="63" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="64"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spring, Junit, Maven, JSON
Spring, Junit, Maven, JSON
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="647">
   <si>
     <t>Main Topic</t>
   </si>
@@ -2189,15 +2189,6 @@
       </rPr>
       <t>images\3_Spring\1_Spring_Security\1_Spring_Security_Hello_World.docx</t>
     </r>
-  </si>
-  <si>
-    <t>Password hashing</t>
-  </si>
-  <si>
-    <t>for Logout</t>
-  </si>
-  <si>
-    <t>Examples</t>
   </si>
   <si>
     <t>http://www.mkyong.com/tutorials/spring-security-tutorials/</t>
@@ -2378,68 +2369,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">If you are using the old JSP 1.2 descriptor, defined by DTD ,for example
-web.xml: 
-&lt;!DOCTYPE web-app PUBLIC
- "-//Sun Microsystems, Inc.//DTD Web Application 2.3//EN"
- "http://java.sun.com/dtd/web-app_2_3.dtd" &gt;
-&lt;web-app&gt; //… &lt;/web-app&gt;
-The EL is disabled or ignored by default, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>you have to enable it manually</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, so that it will outputs the value store in the “msg” model.
-&lt;%@ taglib prefix="c" uri="http://java.sun.com/jsp/jstl/core" %&gt;
-&lt;html&gt;
-&lt;head&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;%@ page isELIgnored="false" %&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-&lt;/head&gt;
-&lt;body&gt;
-           ${msg}
-&lt;/body&gt;
-&lt;/html&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>how to inject an HttpServletRequest into a request-scoped bean?</t>
   </si>
   <si>
@@ -4446,29 +4375,6 @@
     <t>http://fizzylogic.nl/2016/01/24/Make-your-Spring-boot-application-multi-tenant-aware-in-2-steps/</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">If you are using the standard JSP 2.0 descriptor, defined by w3c schema ,for example
-web.xml:
-&lt;web-app id="WebApp_ID" version="2.4"  xmlns="http://java.sun.com/xml/ns/j2ee" 
- xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" 
- xsi:schemaLocation="http://java.sun.com/xml/ns/j2ee  http://java.sun.com/xml/ns/j2ee/web-app_2_4.xsd"&gt;
-//...
-&lt;/web-app&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The EL is enabled by default, and you should see the value stored in the “msg” model, which is “hello world”.</t>
-    </r>
-  </si>
-  <si>
     <t>Spring Cloud released</t>
   </si>
   <si>
@@ -4570,6 +4476,178 @@
 3. add "spring-cloud-config-server", "spring-boot-starter-actuator" dependencies
 4. Add @org.springframework.cloud.config.server.EnableConfigServer annotation to class
 5. create an application.properties (or YAML) with server port, app name and profile</t>
+  </si>
+  <si>
+    <t>AspectJ quick guied - cheat sheet</t>
+  </si>
+  <si>
+    <t>http://www.eclipse.org/aspectj/doc/next/quick5.pdf</t>
+  </si>
+  <si>
+    <t>Spring Security History</t>
+  </si>
+  <si>
+    <t>1. Started as Acegi in 2003
+2. In 2007 brought into spring umbrella as Spring Security
+3. Then onwards Spring Security added as Spring Core technology and under going continuous releases</t>
+  </si>
+  <si>
+    <t>Creating Spring Security application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Create Spring MVC application
+2. </t>
+  </si>
+  <si>
+    <t>What is authentication?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All about determining that who am I? Lot of authentication will be done using LDAP or Active Directory. </t>
+  </si>
+  <si>
+    <t>What is autherization?</t>
+  </si>
+  <si>
+    <t>1. What we can do inside an application. 
+2. Autherization always follows Authentication
+3. First we need to determine who we are and then can determine what we can inside an application</t>
+  </si>
+  <si>
+    <t>1. We need 3 jars - 2 spring security jars, 1 commons-logging jar
+2. spring-security-web
+3. spring-security-config
+4. commons-logging</t>
+  </si>
+  <si>
+    <t>&lt;dependency&gt;
+   &lt;groupId&gt;org.springframework.security&lt;/groupId&gt;   &lt;artifactId&gt;spring-security-web&lt;/artifactId&gt;   &lt;version&gt;4.2.1.RELEASE&lt;/version&gt;
+  &lt;/dependency&gt;
+  &lt;dependency&gt;
+   &lt;groupId&gt;org.springframework.security&lt;/groupId&gt;   &lt;artifactId&gt;spring-security-config&lt;/artifactId&gt;   &lt;version&gt;4.2.1.RELEASE&lt;/version&gt;
+  &lt;/dependency&gt;
+  &lt;dependency&gt;
+   &lt;groupId&gt;commons-logging&lt;/groupId&gt;   &lt;artifactId&gt;commons-logging&lt;/artifactId&gt;   &lt;version&gt;1.2&lt;/version&gt;
+  &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>Enabling Spring Security</t>
+  </si>
+  <si>
+    <t>1. Just like Spring MVC we need to bootstrap our security context. That can be done using below 2 steps:
+a. add org.springframework.web.context.ContextLoaderListener in web.xml as &lt;listener&gt;
+b. add "contextConfigLocation" as context-param in web.xml</t>
+  </si>
+  <si>
+    <t>2. Lastly define Application Entry Point:
+a. add org.springframework.web.filter.DelegatingFilterProxy filter in web.xml
+b. route all requests to this filter using filter-mapping in web.xml</t>
+  </si>
+  <si>
+    <t>Minimal Spring Security Configuration</t>
+  </si>
+  <si>
+    <t>To setup user we must define</t>
+  </si>
+  <si>
+    <t>xmlns that goes in spring-security xml file</t>
+  </si>
+  <si>
+    <t>&lt;beans:beans xmlns="http://www.springframework.org/schema/security"
+ xmlns:beans="http://www.springframework.org/schema/beans" 
+ xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
+ xsi:schemaLocation="http://www.springframework.org/schema/beans http://www.springframework.org/schema/beans/spring-beans-3.0.xsd
+   http://www.springframework.org/schema/security http://www.springframework.org/schema/security/spring-security.xsd"&gt;</t>
+  </si>
+  <si>
+    <t>1. Simplest configuration can be obtained using http tag:
+&lt;http auto-config="true"&gt;
+  &lt;intercept-url pattern="/**" access="hasRole('ROLE_ADMIN')"/&gt;
+ &lt;/http&gt;</t>
+  </si>
+  <si>
+    <t>&lt;authentication-manager&gt;
+  &lt;authentication-provider&gt;
+   &lt;user-service&gt;
+    &lt;user name="admin" password="admin" authorities="ROLE_ADMIN"/&gt;
+   &lt;/user-service&gt;
+  &lt;/authentication-provider&gt;
+ &lt;/authentication-manager&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you are using the old JSP 1.2 descriptor, defined by DTD ,for example
+web.xml: 
+&lt;!DOCTYPE web-app PUBLIC  "-//Sun Microsystems, Inc.//DTD Web Application 2.3//EN"
+ "http://java.sun.com/dtd/web-app_2_3.dtd" &gt;
+&lt;web-app&gt; //… &lt;/web-app&gt;
+The EL is disabled or ignored by default, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you have to enable it manually</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, so that it will outputs the value store in the “msg” model.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enable EL in JSP:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;%@ page isELIgnored="false" %&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solution 2: Change web.xml entry as below:
+web.xml:
+&lt;web-app xmlns="http://java.sun.com/xml/ns/javaee" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
+ xsi:schemaLocation="http://java.sun.com/xml/ns/javaee http://java.sun.com/xml/ns/javaee/web-app_3_0.xsd"
+     version="3.0"&gt;
+//...
+&lt;/web-app&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The EL is enabled by default, and you should see the value stored in the “msg” model, which is “hello world”.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4783,7 +4861,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4977,13 +5055,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5021,10 +5100,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -5041,7 +5120,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5341,7 +5428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5356,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -5393,7 +5480,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="14" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="20"/>
@@ -5421,7 +5508,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="15" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B10" s="15"/>
     </row>
@@ -5433,60 +5520,60 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="15" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="15" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="15" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B15" s="15"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="22" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="15" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -5601,13 +5688,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="73"/>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="79" t="s">
         <v>112</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -5615,7 +5702,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="79"/>
+      <c r="A6" s="80"/>
       <c r="B6" s="7" t="s">
         <v>114</v>
       </c>
@@ -5625,7 +5712,7 @@
         <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60">
@@ -5661,7 +5748,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="86" t="s">
         <v>124</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -5669,7 +5756,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="85"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="7" t="s">
         <v>126</v>
       </c>
@@ -5683,7 +5770,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="86" t="s">
         <v>129</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -5691,7 +5778,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="85"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="7" t="s">
         <v>131</v>
       </c>
@@ -5723,9 +5810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5743,463 +5830,463 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="71" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="32" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="71" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6" s="72"/>
+      <c r="A6" s="72" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="73"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="32" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60">
       <c r="A8" s="32" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="32" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="32" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120">
       <c r="A11" s="32" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="32" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60">
       <c r="A13" s="32" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="32" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45">
       <c r="A16" s="35" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="32" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
       <c r="A18" s="32" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45">
+      <c r="A19" s="84" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="84"/>
+      <c r="B20" s="32" t="s">
         <v>385</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="45">
-      <c r="A19" s="82" t="s">
-        <v>391</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="82"/>
-      <c r="B20" s="32" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45">
       <c r="A21" s="32" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
       <c r="A22" s="32" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="32" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="32" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="75">
       <c r="A25" s="32" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30">
       <c r="A26" s="32" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="83" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120">
       <c r="A28" s="83"/>
       <c r="B28" s="32" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30">
       <c r="A29" s="32" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="32" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
       <c r="A31" s="32" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
       <c r="A32" s="33" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="105">
       <c r="A33" s="57" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90">
       <c r="A34" s="33" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="225">
       <c r="A35" s="35" t="s">
+        <v>408</v>
+      </c>
+      <c r="B35" s="35" t="s">
         <v>412</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30">
       <c r="A36" s="35" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="35" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="35" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="22" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="105">
       <c r="A40" s="48" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="45">
       <c r="A41" s="83" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="210">
       <c r="A42" s="83"/>
       <c r="B42" s="51" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
       <c r="A43" s="52" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="52" t="s">
+        <v>517</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30">
+      <c r="A45" s="88" t="s">
+        <v>519</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="120">
+      <c r="A46" s="88"/>
+      <c r="B46" s="52" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="88"/>
+      <c r="B47" s="27" t="s">
         <v>521</v>
-      </c>
-      <c r="B44" s="52" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="87" t="s">
-        <v>523</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="120">
-      <c r="A46" s="87"/>
-      <c r="B46" s="52" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="87"/>
-      <c r="B47" s="27" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60">
       <c r="A48" s="53" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B48" s="56" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="45" customHeight="1">
-      <c r="A49" s="87" t="s">
-        <v>528</v>
+      <c r="A49" s="88" t="s">
+        <v>524</v>
       </c>
       <c r="B49" s="53" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="87"/>
+      <c r="A50" s="88"/>
       <c r="B50" s="53" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
       <c r="A51" s="53" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="22" customFormat="1" ht="30">
       <c r="A52" s="53" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="B52" s="53" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="45">
       <c r="A53" s="53" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="53" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B54" s="53" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="87" t="s">
-        <v>535</v>
+      <c r="A55" s="88" t="s">
+        <v>531</v>
       </c>
       <c r="B55" s="53" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="60">
-      <c r="A56" s="87"/>
+      <c r="A56" s="88"/>
       <c r="B56" s="53" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="53" t="s">
+        <v>538</v>
+      </c>
+      <c r="B57" s="53" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="45">
+      <c r="A58" s="87" t="s">
+        <v>540</v>
+      </c>
+      <c r="B58" s="55" t="s">
         <v>542</v>
       </c>
-      <c r="B57" s="53" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="86" t="s">
-        <v>544</v>
-      </c>
-      <c r="B58" s="55" t="s">
-        <v>546</v>
-      </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="86"/>
+      <c r="A59" s="87"/>
       <c r="B59" s="54" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
       <c r="A60" s="55" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B60" s="55" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="55" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B61" s="55" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="60">
-      <c r="A62" s="69" t="s">
-        <v>610</v>
-      </c>
-      <c r="B62" s="69" t="s">
-        <v>611</v>
+      <c r="A62" s="68" t="s">
+        <v>605</v>
+      </c>
+      <c r="B62" s="68" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90">
-      <c r="A63" s="69" t="s">
-        <v>612</v>
-      </c>
-      <c r="B63" s="69" t="s">
-        <v>613</v>
+      <c r="A63" s="68" t="s">
+        <v>607</v>
+      </c>
+      <c r="B63" s="68" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -6252,10 +6339,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="71" t="s">
-        <v>316</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="23" t="s">
@@ -6266,139 +6353,139 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="B6" s="72"/>
+      <c r="A6" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="73"/>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="12" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75">
       <c r="A10" s="12" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="88" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="87" t="s">
-        <v>328</v>
-      </c>
       <c r="B11" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="87"/>
+      <c r="A12" s="88"/>
       <c r="B12" s="29" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="75">
       <c r="A13" s="12" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="82" t="s">
-        <v>338</v>
+      <c r="A14" s="84" t="s">
+        <v>334</v>
       </c>
       <c r="B14" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="180">
+      <c r="A15" s="84"/>
+      <c r="B15" s="29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="180">
+      <c r="A16" s="84"/>
+      <c r="B16" s="29" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="82"/>
-      <c r="B15" s="29" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="82"/>
-      <c r="B16" s="29" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="22" customFormat="1" ht="30">
       <c r="A17" s="29" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90">
       <c r="A18" s="12" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="22" customFormat="1" ht="120">
       <c r="A19" s="31" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
       <c r="A20" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="28" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
       <c r="A23" s="30" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -6443,149 +6530,149 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="71" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="59" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="B7" s="72"/>
+      <c r="A7" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="73"/>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="59" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="59" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75">
       <c r="A10" s="59" t="s">
+        <v>569</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1">
+      <c r="A11" s="87" t="s">
+        <v>571</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="87"/>
+      <c r="B12" s="22" t="s">
         <v>573</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" customHeight="1">
-      <c r="A11" s="86" t="s">
-        <v>575</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="86"/>
-      <c r="B12" s="22" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="59" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30">
       <c r="A14" s="60" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="60" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75">
       <c r="A16" s="61" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60">
       <c r="A17" s="62" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75">
       <c r="A18" s="62" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="62" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="62" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
       <c r="A21" s="63" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="105">
       <c r="A22" s="63" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="66" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -6629,93 +6716,93 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="71" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="B7" s="72"/>
+      <c r="A7" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="73"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="22" t="s">
-        <v>606</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>607</v>
+        <v>601</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="22" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="22" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="75">
       <c r="A11" s="22" t="s">
-        <v>616</v>
-      </c>
-      <c r="B11" s="70" t="s">
-        <v>617</v>
+        <v>611</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45">
       <c r="A12" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>619</v>
+        <v>613</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105">
       <c r="A13" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>621</v>
+        <v>615</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120">
       <c r="A14" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="B14" s="69" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="75">
+      <c r="A15" s="89" t="s">
+        <v>619</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30">
+      <c r="A16" s="89"/>
+      <c r="B16" s="69" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="75">
+      <c r="A17" s="70" t="s">
         <v>622</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B17" s="69" t="s">
         <v>623</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="88" t="s">
-        <v>624</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="88"/>
-      <c r="B16" s="70" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="75">
-      <c r="A17" s="89" t="s">
-        <v>627</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -6734,11 +6821,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6756,69 +6843,69 @@
         <v>11</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="22" customFormat="1">
-      <c r="A2" s="71" t="s">
-        <v>497</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="22" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="22" customFormat="1"/>
     <row r="5" spans="1:3">
-      <c r="A5" s="71" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="72"/>
+      <c r="A5" s="72" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" s="73"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="32" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="39" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="75"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="22" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="72"/>
+      <c r="B12" s="73"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="8" t="s">
@@ -6854,94 +6941,94 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="72" t="s">
         <v>290</v>
       </c>
-      <c r="B21" s="72"/>
+      <c r="B21" s="73"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="71" t="s">
-        <v>562</v>
-      </c>
-      <c r="B28" s="72"/>
+      <c r="A28" s="72" t="s">
+        <v>558</v>
+      </c>
+      <c r="B28" s="73"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -6949,43 +7036,58 @@
       <c r="B31" s="22"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="72"/>
+      <c r="B33" s="73"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="71" t="s">
-        <v>598</v>
-      </c>
-      <c r="B36" s="72"/>
+      <c r="A36" s="72" t="s">
+        <v>594</v>
+      </c>
+      <c r="B36" s="73"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>599</v>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="73"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>625</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Materials!A2" display="Up"/>
@@ -7001,9 +7103,10 @@
     <hyperlink ref="B24" r:id="rId9"/>
     <hyperlink ref="B25" r:id="rId10"/>
     <hyperlink ref="B26" r:id="rId11"/>
+    <hyperlink ref="B40" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -7031,21 +7134,21 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="73" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="74"/>
+      <c r="A2" s="74" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="75"/>
     </row>
     <row r="3" spans="1:2" s="22" customFormat="1"/>
     <row r="4" spans="1:2" s="22" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="75"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="81" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -7053,7 +7156,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="81"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -7075,7 +7178,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="45">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="79" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -7083,7 +7186,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
-      <c r="A11" s="79"/>
+      <c r="A11" s="80"/>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -7093,7 +7196,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60">
@@ -7309,7 +7412,7 @@
         <v>74</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
@@ -7361,7 +7464,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="45">
-      <c r="A46" s="79" t="s">
+      <c r="A46" s="80" t="s">
         <v>87</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -7369,19 +7472,19 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="45">
-      <c r="A47" s="79"/>
+      <c r="A47" s="80"/>
       <c r="B47" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60">
-      <c r="A48" s="79"/>
+      <c r="A48" s="80"/>
       <c r="B48" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="45">
-      <c r="A49" s="79" t="s">
+      <c r="A49" s="80" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -7389,19 +7492,19 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="79"/>
+      <c r="A50" s="80"/>
       <c r="B50" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="90">
-      <c r="A51" s="79"/>
+      <c r="A51" s="80"/>
       <c r="B51" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="75">
-      <c r="A52" s="79" t="s">
+      <c r="A52" s="80" t="s">
         <v>95</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -7409,9 +7512,9 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="45">
-      <c r="A53" s="79"/>
+      <c r="A53" s="80"/>
       <c r="B53" s="7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -7419,7 +7522,7 @@
         <v>97</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -7463,7 +7566,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
-      <c r="A60" s="77" t="s">
+      <c r="A60" s="78" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="7" t="s">
@@ -7471,159 +7574,159 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="240">
-      <c r="A61" s="77"/>
+      <c r="A61" s="78"/>
       <c r="B61" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="180">
-      <c r="A62" s="77"/>
+      <c r="A62" s="78"/>
       <c r="B62" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30">
       <c r="A63" s="49" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135">
       <c r="A64" s="24" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150">
       <c r="A65" s="21" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="60">
       <c r="A66" s="34" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30">
       <c r="A67" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="105">
+      <c r="A68" s="77" t="s">
         <v>471</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B68" s="38" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="120">
+      <c r="A69" s="77"/>
+      <c r="B69" s="38" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="75">
+      <c r="A70" s="77"/>
+      <c r="B70" s="38" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="105">
-      <c r="A68" s="76" t="s">
-        <v>475</v>
-      </c>
-      <c r="B68" s="38" t="s">
+    <row r="71" spans="1:2" ht="60">
+      <c r="A71" s="77" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="120">
-      <c r="A69" s="76"/>
-      <c r="B69" s="38" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="75">
-      <c r="A70" s="76"/>
-      <c r="B70" s="38" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="60">
-      <c r="A71" s="76" t="s">
-        <v>476</v>
-      </c>
       <c r="B71" s="46" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60">
-      <c r="A72" s="76"/>
+      <c r="A72" s="77"/>
       <c r="B72" s="46" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30">
       <c r="A73" s="40" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B73" s="41" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60">
       <c r="A74" s="40" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B74" s="41" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="45">
       <c r="A75" s="40" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B75" s="41" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30">
       <c r="A76" s="40" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B76" s="41" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75">
       <c r="A77" s="44" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="42" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B78" s="43" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="45">
       <c r="A79" s="42" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="75" t="s">
-        <v>502</v>
+      <c r="A80" s="76" t="s">
+        <v>498</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="75"/>
+      <c r="A81" s="76"/>
       <c r="B81" s="46" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -7674,10 +7777,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="73"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
@@ -7907,10 +8010,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="72" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="73"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
@@ -7934,11 +8037,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7955,183 +8058,193 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="71" t="s">
+    <row r="2" spans="1:2" s="22" customFormat="1">
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
+    </row>
+    <row r="3" spans="1:2" s="22" customFormat="1"/>
+    <row r="4" spans="1:2" s="22" customFormat="1"/>
+    <row r="5" spans="1:2" s="22" customFormat="1"/>
+    <row r="7" spans="1:2">
+      <c r="A7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="72"/>
-    </row>
-    <row r="4" spans="1:2" ht="90">
-      <c r="A4" s="6" t="s">
+      <c r="B7" s="73"/>
+    </row>
+    <row r="8" spans="1:2" ht="90">
+      <c r="A8" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105">
-      <c r="A5" s="6" t="s">
+    <row r="9" spans="1:2" ht="105">
+      <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="135">
-      <c r="A6" s="10" t="s">
+    <row r="10" spans="1:2" ht="135">
+      <c r="A10" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
-        <v>197</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30">
+      <c r="A12" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="8" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>199</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
       <c r="A21" s="6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30">
       <c r="A24" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30">
+      <c r="A25" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30">
+      <c r="A28" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A5" display="Topics"/>
@@ -8145,9 +8258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8166,10 +8279,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="22" customFormat="1">
-      <c r="A2" s="71" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="72"/>
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
     </row>
     <row r="3" spans="1:2" s="22" customFormat="1">
       <c r="A3" s="8"/>
@@ -8180,10 +8293,10 @@
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="B5" s="72"/>
+      <c r="A5" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="73"/>
     </row>
     <row r="6" spans="1:2" ht="75">
       <c r="A6" s="36" t="s">
@@ -8194,263 +8307,268 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="120">
-      <c r="A7" s="79" t="s">
-        <v>310</v>
+      <c r="A7" s="80" t="s">
+        <v>307</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="240">
-      <c r="A8" s="79"/>
+      <c r="A8" s="80"/>
       <c r="B8" s="12" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60">
-      <c r="A9" s="76" t="s">
-        <v>325</v>
+      <c r="A9" s="77" t="s">
+        <v>322</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="255">
-      <c r="A10" s="76"/>
-      <c r="B10" s="67" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="120">
-      <c r="A11" s="76"/>
-      <c r="B11" s="67" t="s">
-        <v>605</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="120">
+      <c r="A10" s="77"/>
+      <c r="B10" s="71" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135">
+      <c r="A11" s="77"/>
+      <c r="B11" s="71" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="150">
-      <c r="A12" s="82" t="s">
-        <v>444</v>
+      <c r="A12" s="84" t="s">
+        <v>440</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="22" customFormat="1" ht="105">
-      <c r="A13" s="82"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="36" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="84" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60">
+      <c r="A15" s="84"/>
+      <c r="B15" s="64" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="45">
+      <c r="A16" s="84"/>
+      <c r="B16" s="36" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30">
+      <c r="A17" s="84" t="s">
         <v>422</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B17" s="36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60">
-      <c r="A15" s="82"/>
-      <c r="B15" s="64" t="s">
+    <row r="18" spans="1:2" ht="135">
+      <c r="A18" s="84"/>
+      <c r="B18" s="36" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45">
-      <c r="A16" s="82"/>
-      <c r="B16" s="36" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="84"/>
+      <c r="B19" s="36" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="82" t="s">
+    <row r="20" spans="1:2" ht="45">
+      <c r="A20" s="84"/>
+      <c r="B20" s="36" t="s">
         <v>426</v>
       </c>
-      <c r="B17" s="36" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="30">
+      <c r="A21" s="84"/>
+      <c r="B21" s="36" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="135">
-      <c r="A18" s="82"/>
-      <c r="B18" s="36" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="82"/>
-      <c r="B19" s="36" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="82"/>
-      <c r="B20" s="36" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="82"/>
-      <c r="B21" s="36" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
       <c r="A22" s="83" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="45">
       <c r="A23" s="83"/>
       <c r="B23" s="36" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30">
       <c r="A24" s="83"/>
       <c r="B24" s="36" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="45">
       <c r="A25" s="83"/>
       <c r="B25" s="36" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="45">
       <c r="A26" s="83"/>
       <c r="B26" s="36" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="84" t="s">
+        <v>434</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="165">
+      <c r="A28" s="84"/>
+      <c r="B28" s="36" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30">
+      <c r="A29" s="84"/>
+      <c r="B29" s="36" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="82" t="s">
-        <v>438</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="165">
-      <c r="A28" s="82"/>
-      <c r="B28" s="36" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="82"/>
-      <c r="B29" s="36" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30">
       <c r="A30" s="50" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="60">
       <c r="A31" s="36" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
       <c r="A32" s="36" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="75">
       <c r="A33" s="36" t="s">
+        <v>446</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30">
+      <c r="A34" s="84" t="s">
+        <v>448</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="75">
+      <c r="A35" s="84"/>
+      <c r="B35" s="36" t="s">
         <v>450</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="82" t="s">
-        <v>452</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="75">
-      <c r="A35" s="82"/>
-      <c r="B35" s="36" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120">
       <c r="A36" s="36" t="s">
+        <v>451</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="84" t="s">
+        <v>453</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30">
+      <c r="A38" s="84"/>
+      <c r="B38" s="36" t="s">
         <v>455</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="82" t="s">
-        <v>457</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30">
-      <c r="A38" s="82"/>
-      <c r="B38" s="36" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135">
       <c r="A39" s="36" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="82" t="s">
-        <v>457</v>
+      <c r="A40" s="84" t="s">
+        <v>453</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="60">
-      <c r="A41" s="82"/>
+      <c r="A41" s="84"/>
       <c r="B41" s="36" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30">
       <c r="A42" s="83" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="60">
       <c r="A43" s="83"/>
       <c r="B43" s="65" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A12:A13"/>
@@ -8459,11 +8577,6 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -8498,10 +8611,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="73"/>
     </row>
     <row r="4" spans="1:2" ht="60">
       <c r="A4" s="8" t="s">
@@ -8552,7 +8665,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="80" t="s">
         <v>248</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -8560,25 +8673,25 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="79"/>
+      <c r="A11" s="80"/>
       <c r="B11" s="7" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="79"/>
+      <c r="A12" s="80"/>
       <c r="B12" s="7" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>252</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="85"/>
     </row>
     <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="80" t="s">
         <v>253</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -8586,13 +8699,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="79"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="7" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
-      <c r="A16" s="79"/>
+      <c r="A16" s="80"/>
       <c r="B16" s="7" t="s">
         <v>256</v>
       </c>
@@ -8622,7 +8735,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="80" t="s">
         <v>263</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -8630,7 +8743,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="79"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="7" t="s">
         <v>265</v>
       </c>
@@ -8708,7 +8821,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="80" t="s">
         <v>284</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -8716,13 +8829,13 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="79"/>
+      <c r="A32" s="80"/>
       <c r="B32" s="7" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="79"/>
+      <c r="A33" s="80"/>
       <c r="B33" s="7" t="s">
         <v>287</v>
       </c>
@@ -8754,17 +8867,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B7"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" customWidth="1"/>
-    <col min="2" max="2" width="121.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="133.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8775,52 +8888,125 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="73"/>
+    </row>
     <row r="3" spans="1:2" s="22" customFormat="1"/>
-    <row r="8" spans="1:2">
-      <c r="B8" s="15"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="71" t="s">
-        <v>297</v>
-      </c>
-      <c r="B10" s="72"/>
+    <row r="6" spans="1:2">
+      <c r="A6" s="72" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="73"/>
+    </row>
+    <row r="7" spans="1:2" s="22" customFormat="1">
+      <c r="A7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="22" customFormat="1" ht="45">
+      <c r="A8" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="22" t="s">
+        <v>628</v>
+      </c>
+      <c r="B10" s="71" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>293</v>
-      </c>
-      <c r="B11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="71" t="s">
-        <v>291</v>
-      </c>
-      <c r="B15" s="72"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>296</v>
+      <c r="A11" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="B11" s="71" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45">
+      <c r="A12" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="B12" s="71" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="60">
+      <c r="A13" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="71" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="165">
+      <c r="A14" s="90"/>
+      <c r="B14" s="71" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45">
+      <c r="A15" s="91" t="s">
+        <v>636</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="45">
+      <c r="A16" s="91"/>
+      <c r="B16" s="71" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="22" customFormat="1" ht="75">
+      <c r="A17" s="92" t="s">
+        <v>641</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="60">
+      <c r="A18" s="70" t="s">
+        <v>639</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="105">
+      <c r="A19" s="70" t="s">
+        <v>640</v>
+      </c>
+      <c r="B19" s="71" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A10:B10"/>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>

<commit_message>
Spring Boot MongoDB Query logging
Spring Boot MongoDB Query logging
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="858">
   <si>
     <t>Main Topic</t>
   </si>
@@ -5479,6 +5479,18 @@
   </si>
   <si>
     <t>grabs an instance of EntityManagerFactory and injects into our code</t>
+  </si>
+  <si>
+    <t>logging.level.org.springframework.data.mongodb.core.MongoTemplate=DEBUG</t>
+  </si>
+  <si>
+    <t>To display queries while executing against mongo db</t>
+  </si>
+  <si>
+    <t>To display JPA queries</t>
+  </si>
+  <si>
+    <t>spring.jpa.show-sql=true</t>
   </si>
 </sst>
 </file>
@@ -5692,7 +5704,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5939,6 +5951,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5976,21 +5991,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -6568,13 +6583,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="88"/>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="96" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -6582,7 +6597,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="96"/>
+      <c r="A6" s="97"/>
       <c r="B6" s="5" t="s">
         <v>108</v>
       </c>
@@ -6628,7 +6643,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="105" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -6636,7 +6651,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="104"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="5" t="s">
         <v>120</v>
       </c>
@@ -6650,7 +6665,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="105" t="s">
         <v>123</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -6658,7 +6673,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="104"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="5" t="s">
         <v>125</v>
       </c>
@@ -6696,11 +6711,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6718,10 +6733,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>411</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="29" t="s">
@@ -6732,10 +6747,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="87" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="87"/>
+      <c r="B6" s="88"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="29" t="s">
@@ -6896,7 +6911,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="100" t="s">
         <v>392</v>
       </c>
       <c r="B27" s="29" t="s">
@@ -6904,7 +6919,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="120">
-      <c r="A28" s="98"/>
+      <c r="A28" s="100"/>
       <c r="B28" s="29" t="s">
         <v>393</v>
       </c>
@@ -7006,7 +7021,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="45">
-      <c r="A41" s="98" t="s">
+      <c r="A41" s="100" t="s">
         <v>507</v>
       </c>
       <c r="B41" s="48" t="s">
@@ -7014,7 +7029,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="210">
-      <c r="A42" s="98"/>
+      <c r="A42" s="100"/>
       <c r="B42" s="48" t="s">
         <v>506</v>
       </c>
@@ -7036,7 +7051,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="98" t="s">
         <v>512</v>
       </c>
       <c r="B45" s="49" t="s">
@@ -7044,13 +7059,13 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="120">
-      <c r="A46" s="97"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="49" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="97"/>
+      <c r="A47" s="98"/>
       <c r="B47" s="24" t="s">
         <v>514</v>
       </c>
@@ -7064,7 +7079,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="45" customHeight="1">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="98" t="s">
         <v>517</v>
       </c>
       <c r="B49" s="50" t="s">
@@ -7072,7 +7087,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="97"/>
+      <c r="A50" s="98"/>
       <c r="B50" s="50" t="s">
         <v>519</v>
       </c>
@@ -7110,7 +7125,7 @@
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="97" t="s">
+      <c r="A55" s="98" t="s">
         <v>524</v>
       </c>
       <c r="B55" s="50" t="s">
@@ -7118,7 +7133,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="60">
-      <c r="A56" s="97"/>
+      <c r="A56" s="98"/>
       <c r="B56" s="50" t="s">
         <v>530</v>
       </c>
@@ -7132,7 +7147,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="104" t="s">
         <v>533</v>
       </c>
       <c r="B58" s="52" t="s">
@@ -7140,7 +7155,7 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="101"/>
+      <c r="A59" s="104"/>
       <c r="B59" s="51" t="s">
         <v>534</v>
       </c>
@@ -7175,6 +7190,22 @@
       </c>
       <c r="B63" s="65" t="s">
         <v>601</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="86" t="s">
+        <v>855</v>
+      </c>
+      <c r="B64" s="86" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="86" t="s">
+        <v>856</v>
+      </c>
+      <c r="B65" s="86" t="s">
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -7227,10 +7258,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
@@ -7241,10 +7272,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="87" t="s">
         <v>308</v>
       </c>
-      <c r="B6" s="87"/>
+      <c r="B6" s="88"/>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="9" t="s">
@@ -7279,7 +7310,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="98" t="s">
         <v>318</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -7287,7 +7318,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="97"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="26" t="s">
         <v>320</v>
       </c>
@@ -7418,10 +7449,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>411</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="56" t="s">
@@ -7432,10 +7463,10 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="87" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="87"/>
+      <c r="B7" s="88"/>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="56" t="s">
@@ -7462,7 +7493,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" customHeight="1">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="104" t="s">
         <v>564</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -7470,7 +7501,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="101"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="19" t="s">
         <v>566</v>
       </c>
@@ -7604,16 +7635,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>411</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="87" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="87"/>
+      <c r="B7" s="88"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="19" t="s">
@@ -7672,7 +7703,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="106" t="s">
         <v>612</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -7680,7 +7711,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="105"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="66" t="s">
         <v>614</v>
       </c>
@@ -7735,10 +7766,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="19" customFormat="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>486</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
@@ -7750,10 +7781,10 @@
     </row>
     <row r="4" spans="1:3" s="19" customFormat="1"/>
     <row r="5" spans="1:3">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="87" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="87"/>
+      <c r="B5" s="88"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="29" t="s">
@@ -7776,10 +7807,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="89"/>
+      <c r="B9" s="90"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="19" t="s">
@@ -7790,10 +7821,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="87"/>
+      <c r="B12" s="88"/>
     </row>
     <row r="13" spans="1:3" s="19" customFormat="1">
       <c r="A13" s="6" t="s">
@@ -7860,10 +7891,10 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="87" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="87"/>
+      <c r="B22" s="88"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="19" t="s">
@@ -7909,10 +7940,10 @@
       <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="86" t="s">
+      <c r="A29" s="87" t="s">
         <v>640</v>
       </c>
-      <c r="B29" s="87"/>
+      <c r="B29" s="88"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="67" t="s">
@@ -7924,10 +7955,10 @@
     </row>
     <row r="31" spans="1:2" s="19" customFormat="1"/>
     <row r="32" spans="1:2">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="87" t="s">
         <v>551</v>
       </c>
-      <c r="B32" s="87"/>
+      <c r="B32" s="88"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
@@ -7950,10 +7981,10 @@
       <c r="B35" s="19"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="86" t="s">
+      <c r="A37" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="87"/>
+      <c r="B37" s="88"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="19" t="s">
@@ -7964,10 +7995,10 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="86" t="s">
+      <c r="A40" s="87" t="s">
         <v>587</v>
       </c>
-      <c r="B40" s="87"/>
+      <c r="B40" s="88"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="19" t="s">
@@ -7978,10 +8009,10 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="91"/>
+      <c r="B43" s="92"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="19" t="s">
@@ -8051,10 +8082,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="90"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="19" t="s">
@@ -8076,10 +8107,10 @@
     <row r="6" spans="1:2" s="19" customFormat="1"/>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="89" t="s">
         <v>663</v>
       </c>
-      <c r="B8" s="89"/>
+      <c r="B8" s="90"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="19" t="s">
@@ -8098,13 +8129,13 @@
     <row r="16" spans="1:2" s="19" customFormat="1"/>
     <row r="17" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="18" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="89"/>
+      <c r="B18" s="90"/>
     </row>
     <row r="19" spans="1:2" ht="45">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="96" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -8112,7 +8143,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="96"/>
+      <c r="A20" s="97"/>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
@@ -8390,7 +8421,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="45">
-      <c r="A55" s="96" t="s">
+      <c r="A55" s="97" t="s">
         <v>81</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -8398,19 +8429,19 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="45">
-      <c r="A56" s="96"/>
+      <c r="A56" s="97"/>
       <c r="B56" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="96"/>
+      <c r="A57" s="97"/>
       <c r="B57" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="96" t="s">
+      <c r="A58" s="97" t="s">
         <v>85</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -8418,19 +8449,19 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
-      <c r="A59" s="96"/>
+      <c r="A59" s="97"/>
       <c r="B59" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90">
-      <c r="A60" s="96"/>
+      <c r="A60" s="97"/>
       <c r="B60" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="75">
-      <c r="A61" s="96" t="s">
+      <c r="A61" s="97" t="s">
         <v>89</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -8438,7 +8469,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="45">
-      <c r="A62" s="96"/>
+      <c r="A62" s="97"/>
       <c r="B62" s="5" t="s">
         <v>322</v>
       </c>
@@ -8492,7 +8523,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -8500,13 +8531,13 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="240">
-      <c r="A70" s="94"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="180">
-      <c r="A71" s="94"/>
+      <c r="A71" s="95"/>
       <c r="B71" s="5" t="s">
         <v>105</v>
       </c>
@@ -8560,7 +8591,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" ht="105">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="94" t="s">
         <v>465</v>
       </c>
       <c r="B78" s="35" t="s">
@@ -8568,19 +8599,19 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="120">
-      <c r="A79" s="93"/>
+      <c r="A79" s="94"/>
       <c r="B79" s="35" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75">
-      <c r="A80" s="93"/>
+      <c r="A80" s="94"/>
       <c r="B80" s="35" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="60">
-      <c r="A81" s="93" t="s">
+      <c r="A81" s="94" t="s">
         <v>466</v>
       </c>
       <c r="B81" s="43" t="s">
@@ -8588,7 +8619,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" ht="60">
-      <c r="A82" s="93"/>
+      <c r="A82" s="94"/>
       <c r="B82" s="43" t="s">
         <v>489</v>
       </c>
@@ -8650,7 +8681,7 @@
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="92" t="s">
+      <c r="A90" s="93" t="s">
         <v>491</v>
       </c>
       <c r="B90" s="43" t="s">
@@ -8658,7 +8689,7 @@
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="92"/>
+      <c r="A91" s="93"/>
       <c r="B91" s="43" t="s">
         <v>493</v>
       </c>
@@ -8711,10 +8742,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="88"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
@@ -8924,7 +8955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
@@ -8944,10 +8975,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="87" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="87"/>
+      <c r="B3" s="88"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
@@ -9009,10 +9040,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="76"/>
@@ -9030,10 +9061,10 @@
       <c r="A7" s="76"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="87" t="s">
         <v>668</v>
       </c>
-      <c r="B8" s="87"/>
+      <c r="B8" s="88"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="76"/>
@@ -9060,10 +9091,10 @@
       <c r="A16" s="76"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="87" t="s">
         <v>656</v>
       </c>
-      <c r="B18" s="87"/>
+      <c r="B18" s="88"/>
     </row>
     <row r="19" spans="1:2" ht="90">
       <c r="A19" s="75" t="s">
@@ -9234,10 +9265,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="86" t="s">
+      <c r="A41" s="87" t="s">
         <v>657</v>
       </c>
-      <c r="B41" s="87"/>
+      <c r="B41" s="88"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="46" t="s">
@@ -9248,7 +9279,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="98" t="s">
         <v>661</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -9256,7 +9287,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="97"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="19" t="s">
         <v>693</v>
       </c>
@@ -9462,7 +9493,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="120">
-      <c r="A70" s="97" t="s">
+      <c r="A70" s="98" t="s">
         <v>736</v>
       </c>
       <c r="B70" s="80" t="s">
@@ -9470,13 +9501,13 @@
       </c>
     </row>
     <row r="71" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A71" s="97"/>
+      <c r="A71" s="98"/>
       <c r="B71" s="80" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60">
-      <c r="A72" s="97" t="s">
+      <c r="A72" s="98" t="s">
         <v>744</v>
       </c>
       <c r="B72" s="80" t="s">
@@ -9484,7 +9515,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" ht="60">
-      <c r="A73" s="97"/>
+      <c r="A73" s="98"/>
       <c r="B73" s="80" t="s">
         <v>746</v>
       </c>
@@ -9610,7 +9641,7 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="97" t="s">
+      <c r="A89" s="98" t="s">
         <v>777</v>
       </c>
       <c r="B89" s="83" t="s">
@@ -9618,13 +9649,13 @@
       </c>
     </row>
     <row r="90" spans="1:2" ht="90">
-      <c r="A90" s="97"/>
+      <c r="A90" s="98"/>
       <c r="B90" s="80" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75">
-      <c r="A91" s="97"/>
+      <c r="A91" s="98"/>
       <c r="B91" s="80" t="s">
         <v>779</v>
       </c>
@@ -9779,7 +9810,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="60">
-      <c r="A111" s="97" t="s">
+      <c r="A111" s="98" t="s">
         <v>818</v>
       </c>
       <c r="B111" s="81" t="s">
@@ -9787,7 +9818,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="60">
-      <c r="A112" s="97"/>
+      <c r="A112" s="98"/>
       <c r="B112" s="81" t="s">
         <v>820</v>
       </c>
@@ -9888,10 +9919,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>647</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="6" t="s">
@@ -9914,10 +9945,10 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="87" t="s">
         <v>648</v>
       </c>
-      <c r="B7" s="87"/>
+      <c r="B7" s="88"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
       <c r="A8" s="6"/>
@@ -9940,10 +9971,10 @@
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="87" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="87"/>
+      <c r="B13" s="88"/>
     </row>
     <row r="14" spans="1:2" ht="75">
       <c r="A14" s="33" t="s">
@@ -9954,7 +9985,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="120">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="97" t="s">
         <v>301</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -9962,13 +9993,13 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="240">
-      <c r="A16" s="96"/>
+      <c r="A16" s="97"/>
       <c r="B16" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="94" t="s">
         <v>316</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -9976,13 +10007,13 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="120">
-      <c r="A18" s="93"/>
+      <c r="A18" s="94"/>
       <c r="B18" s="68" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135">
-      <c r="A19" s="93"/>
+      <c r="A19" s="94"/>
       <c r="B19" s="84" t="s">
         <v>638</v>
       </c>
@@ -10054,7 +10085,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="100" t="s">
         <v>422</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -10062,25 +10093,25 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="98"/>
+      <c r="A31" s="100"/>
       <c r="B31" s="33" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="98"/>
+      <c r="A32" s="100"/>
       <c r="B32" s="33" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="98"/>
+      <c r="A33" s="100"/>
       <c r="B33" s="33" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="98"/>
+      <c r="A34" s="100"/>
       <c r="B34" s="33" t="s">
         <v>427</v>
       </c>
@@ -10196,7 +10227,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="98" t="s">
+      <c r="A50" s="100" t="s">
         <v>589</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10204,16 +10235,16 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="60">
-      <c r="A51" s="98"/>
+      <c r="A51" s="100"/>
       <c r="B51" s="62" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="86" t="s">
+      <c r="A53" s="87" t="s">
         <v>837</v>
       </c>
-      <c r="B53" s="87"/>
+      <c r="B53" s="88"/>
     </row>
     <row r="54" spans="1:2" ht="45">
       <c r="A54" s="84" t="s">
@@ -10265,12 +10296,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A48:A49"/>
@@ -10280,6 +10305,12 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -10314,10 +10345,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="87"/>
+      <c r="B3" s="88"/>
     </row>
     <row r="4" spans="1:2" ht="60">
       <c r="A4" s="6" t="s">
@@ -10368,7 +10399,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>242</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -10376,25 +10407,25 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="96"/>
+      <c r="A11" s="97"/>
       <c r="B11" s="5" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="96"/>
+      <c r="A12" s="97"/>
       <c r="B12" s="5" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="101"/>
     </row>
     <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>247</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -10402,13 +10433,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="96"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
-      <c r="A16" s="96"/>
+      <c r="A16" s="97"/>
       <c r="B16" s="5" t="s">
         <v>250</v>
       </c>
@@ -10438,7 +10469,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="96" t="s">
+      <c r="A20" s="97" t="s">
         <v>257</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -10446,7 +10477,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="96"/>
+      <c r="A21" s="97"/>
       <c r="B21" s="5" t="s">
         <v>259</v>
       </c>
@@ -10524,7 +10555,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="97" t="s">
         <v>278</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -10532,13 +10563,13 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="96"/>
+      <c r="A32" s="97"/>
       <c r="B32" s="5" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="96"/>
+      <c r="A33" s="97"/>
       <c r="B33" s="5" t="s">
         <v>281</v>
       </c>
@@ -10592,10 +10623,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>647</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1"/>
     <row r="5" spans="1:2">
@@ -10612,10 +10643,10 @@
       <c r="A9" s="69"/>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="87" t="s">
         <v>651</v>
       </c>
-      <c r="B10" s="87"/>
+      <c r="B10" s="88"/>
     </row>
     <row r="11" spans="1:2" s="19" customFormat="1">
       <c r="A11" s="103" t="s">
@@ -10626,13 +10657,13 @@
       </c>
     </row>
     <row r="12" spans="1:2" s="19" customFormat="1">
-      <c r="A12" s="101"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="12" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="104" t="s">
         <v>654</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -10640,7 +10671,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" s="19" customFormat="1">
-      <c r="A14" s="101"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="12" t="s">
         <v>646</v>
       </c>
@@ -10667,10 +10698,10 @@
       <c r="A21" s="69"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="87" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="87"/>
+      <c r="B22" s="88"/>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1">
       <c r="A23" s="69" t="s">
@@ -10721,7 +10752,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="60">
-      <c r="A29" s="98" t="s">
+      <c r="A29" s="100" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="68" t="s">
@@ -10729,7 +10760,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="165">
-      <c r="A30" s="98"/>
+      <c r="A30" s="100"/>
       <c r="B30" s="68" t="s">
         <v>627</v>
       </c>
@@ -10797,7 +10828,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="104" t="s">
         <v>676</v>
       </c>
       <c r="B39" s="73" t="s">
@@ -10805,13 +10836,13 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="120">
-      <c r="A40" s="101"/>
+      <c r="A40" s="104"/>
       <c r="B40" s="73" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="98" t="s">
         <v>680</v>
       </c>
       <c r="B41" s="73" t="s">
@@ -10819,13 +10850,13 @@
       </c>
     </row>
     <row r="42" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A42" s="97"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="73" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="98" t="s">
         <v>677</v>
       </c>
       <c r="B43" s="73" t="s">
@@ -10833,13 +10864,13 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="97"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="73" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="75">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="98" t="s">
         <v>686</v>
       </c>
       <c r="B45" s="73" t="s">
@@ -10847,7 +10878,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="60">
-      <c r="A46" s="97"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="73" t="s">
         <v>688</v>
       </c>
@@ -10870,17 +10901,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>

<commit_message>
Spring, Scala, Todo, Design Patterns
Spring, Scala, Todo, Design Patterns
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -6256,21 +6256,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -7150,7 +7150,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="104" t="s">
         <v>381</v>
       </c>
       <c r="B20" s="54" t="s">
@@ -7158,7 +7158,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="105"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="29" t="s">
         <v>379</v>
       </c>
@@ -7212,7 +7212,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>392</v>
       </c>
       <c r="B28" s="29" t="s">
@@ -7220,7 +7220,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="120">
-      <c r="A29" s="104"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="29" t="s">
         <v>393</v>
       </c>
@@ -7322,7 +7322,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="45">
-      <c r="A42" s="104" t="s">
+      <c r="A42" s="105" t="s">
         <v>506</v>
       </c>
       <c r="B42" s="48" t="s">
@@ -7330,7 +7330,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="210">
-      <c r="A43" s="104"/>
+      <c r="A43" s="105"/>
       <c r="B43" s="48" t="s">
         <v>505</v>
       </c>
@@ -7448,7 +7448,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="45">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="109" t="s">
         <v>532</v>
       </c>
       <c r="B59" s="52" t="s">
@@ -7456,7 +7456,7 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="107"/>
+      <c r="A60" s="109"/>
       <c r="B60" s="51" t="s">
         <v>533</v>
       </c>
@@ -7641,7 +7641,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="104" t="s">
         <v>328</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -7649,13 +7649,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="105"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="26" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="105"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="26" t="s">
         <v>344</v>
       </c>
@@ -7802,7 +7802,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" customHeight="1">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="109" t="s">
         <v>563</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -7810,7 +7810,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="107"/>
+      <c r="A12" s="109"/>
       <c r="B12" s="19" t="s">
         <v>565</v>
       </c>
@@ -8512,8 +8512,8 @@
   <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10476,7 +10476,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="150">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="104" t="s">
         <v>433</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -10484,13 +10484,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A21" s="105"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="33" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="104" t="s">
         <v>411</v>
       </c>
       <c r="B22" s="33" t="s">
@@ -10498,19 +10498,19 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="60">
-      <c r="A23" s="105"/>
+      <c r="A23" s="104"/>
       <c r="B23" s="61" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="105"/>
+      <c r="A24" s="104"/>
       <c r="B24" s="33" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
-      <c r="A25" s="105" t="s">
+      <c r="A25" s="104" t="s">
         <v>415</v>
       </c>
       <c r="B25" s="33" t="s">
@@ -10518,31 +10518,31 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="135">
-      <c r="A26" s="105"/>
+      <c r="A26" s="104"/>
       <c r="B26" s="33" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="105"/>
+      <c r="A27" s="104"/>
       <c r="B27" s="33" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="105"/>
+      <c r="A28" s="104"/>
       <c r="B28" s="33" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="105"/>
+      <c r="A29" s="104"/>
       <c r="B29" s="33" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="105" t="s">
         <v>421</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -10550,31 +10550,31 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="104"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="33" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="104"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="33" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="104"/>
+      <c r="A33" s="105"/>
       <c r="B33" s="33" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="104"/>
+      <c r="A34" s="105"/>
       <c r="B34" s="33" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30">
-      <c r="A35" s="105" t="s">
+      <c r="A35" s="104" t="s">
         <v>427</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -10582,13 +10582,13 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="165">
-      <c r="A36" s="105"/>
+      <c r="A36" s="104"/>
       <c r="B36" s="33" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="105"/>
+      <c r="A37" s="104"/>
       <c r="B37" s="33" t="s">
         <v>430</v>
       </c>
@@ -10626,7 +10626,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="30">
-      <c r="A42" s="105" t="s">
+      <c r="A42" s="104" t="s">
         <v>441</v>
       </c>
       <c r="B42" s="33" t="s">
@@ -10634,7 +10634,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="75">
-      <c r="A43" s="105"/>
+      <c r="A43" s="104"/>
       <c r="B43" s="33" t="s">
         <v>443</v>
       </c>
@@ -10648,7 +10648,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="104" t="s">
         <v>446</v>
       </c>
       <c r="B45" s="33" t="s">
@@ -10656,7 +10656,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="105"/>
+      <c r="A46" s="104"/>
       <c r="B46" s="33" t="s">
         <v>448</v>
       </c>
@@ -10670,7 +10670,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="104" t="s">
         <v>446</v>
       </c>
       <c r="B48" s="33" t="s">
@@ -10678,13 +10678,13 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="60">
-      <c r="A49" s="105"/>
+      <c r="A49" s="104"/>
       <c r="B49" s="33" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="104" t="s">
+      <c r="A50" s="105" t="s">
         <v>588</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10692,7 +10692,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="60">
-      <c r="A51" s="104"/>
+      <c r="A51" s="105"/>
       <c r="B51" s="62" t="s">
         <v>590</v>
       </c>
@@ -10753,12 +10753,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A48:A49"/>
@@ -10768,6 +10762,12 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -11106,7 +11106,7 @@
       <c r="B10" s="93"/>
     </row>
     <row r="11" spans="1:2" s="19" customFormat="1">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="108" t="s">
         <v>654</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -11114,13 +11114,13 @@
       </c>
     </row>
     <row r="12" spans="1:2" s="19" customFormat="1">
-      <c r="A12" s="107"/>
+      <c r="A12" s="109"/>
       <c r="B12" s="12" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="109" t="s">
         <v>653</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -11128,7 +11128,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" s="19" customFormat="1">
-      <c r="A14" s="107"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="12" t="s">
         <v>645</v>
       </c>
@@ -11209,7 +11209,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="60">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="105" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="68" t="s">
@@ -11217,13 +11217,13 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="165">
-      <c r="A30" s="104"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="68" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="107" t="s">
         <v>627</v>
       </c>
       <c r="B31" s="68" t="s">
@@ -11231,7 +11231,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="45">
-      <c r="A32" s="108"/>
+      <c r="A32" s="107"/>
       <c r="B32" s="68" t="s">
         <v>629</v>
       </c>
@@ -11285,7 +11285,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="107" t="s">
+      <c r="A39" s="109" t="s">
         <v>675</v>
       </c>
       <c r="B39" s="73" t="s">
@@ -11293,7 +11293,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="120">
-      <c r="A40" s="107"/>
+      <c r="A40" s="109"/>
       <c r="B40" s="73" t="s">
         <v>672</v>
       </c>
@@ -11358,17 +11358,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>

<commit_message>
Todo, Spring, Unit Testing
Todo, Spring, Unit Testing
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="912">
   <si>
     <t>Main Topic</t>
   </si>
@@ -2595,18 +2595,12 @@
     <t xml:space="preserve"> @SpringBootApplication</t>
   </si>
   <si>
-    <t>A convinience annotation that wraps commonly used spring annotations with spring boot</t>
-  </si>
-  <si>
     <t>1. Spring configuration on start up
 2. Auto Configures framework
 3. Scans project for spring components</t>
   </si>
   <si>
     <t>SpringApplication.run(…)</t>
-  </si>
-  <si>
-    <t>Starts spring, creates spring context, applies annotations, and setup container</t>
   </si>
   <si>
     <r>
@@ -2664,9 +2658,6 @@
   </si>
   <si>
     <t xml:space="preserve">static content (like html, properties etc files) will go to these locations </t>
-  </si>
-  <si>
-    <t>1. src/main/resources -&gt; public folder</t>
   </si>
   <si>
     <t>SpringBootPractice</t>
@@ -5534,98 +5525,6 @@
     <t xml:space="preserve"> @SpringBootApplication is a convenience annotation that adds all of the following:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@Configuration:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tags the class as a source of bean definitions for the application context.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@EnableAutoConfiguration:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tells Spring Boot to start adding beans based on classpath settings, other beans, and various property settings.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@EnableWebMvc:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Normally you would add @EnableWebMvc for a Spring MVC app, but Spring Boot adds it automatically when it sees spring-webmvc on the classpath. This flags the application as a web application and activates key behaviors such as setting up a DispatcherServlet.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@ComponentScan:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tells Spring to look for other components, configurations, and services in the packages specified in basePackages attribute, allowing it to find the controllers.</t>
-    </r>
-  </si>
-  <si>
     <t>Hello World Spring doc URL</t>
   </si>
   <si>
@@ -5741,6 +5640,185 @@
   <si>
     <t>Resource resource = new ClassPathResource("fileName.csv");
 File file = resource.getFile(); // this will throw an exception, handle it</t>
+  </si>
+  <si>
+    <t>A convinience annotation that wraps commonly used spring annotations with spring boot.
+Scans our project for spring components, and wires up most of the spring libraries we want to use by enabling spring auto-configuration.</t>
+  </si>
+  <si>
+    <t>Starts spring, creates spring context, applies annotations, and setup container.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Dependency Management structure is known as </t>
+  </si>
+  <si>
+    <t>BOM (Bill Of Material)</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>Intelligent collection of dependencies</t>
+  </si>
+  <si>
+    <t>How BOM works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When we added spring-boot-starter-parent to our build, parent will brought in all dependencies. The starter parent also setup some defaults that also useful for the project like plugins, Java support, resource filtering and so on. </t>
+  </si>
+  <si>
+    <t>Spring Boot CLI</t>
+  </si>
+  <si>
+    <t>Sprint Boot CLI can initialize a project just like start.spring.io does. Infact it actually does calling same API that start.spring.io uses but it is another way of using spring initializer from the command line</t>
+  </si>
+  <si>
+    <t>Create spring boot project using spring boot cli</t>
+  </si>
+  <si>
+    <t>E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects&gt;E:\Backup\JavaPrep\Spring\Spring_Boot\spring-1.5.3.RELEASE\bin\spring.bat init --dependencies=web mySpringBootAppFromCLI
+Using service at https://start.spring.io
+Project extracted to 'E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects\mySpringBootAppFromCLI'</t>
+  </si>
+  <si>
+    <t>Installing Spring Boot CLI</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. download it from 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://docs.spring.io/spring-boot/docs/current/reference/html/getting-started-installing-spring-boot.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. download spring-boot-cli-1.5.3.RELEASE-bin.zip and unzip it
+3. go to bin directory and run "spring.bat --version"
+4. we should see following output</t>
+    </r>
+  </si>
+  <si>
+    <t>E:\Backup\JavaPrep\Spring\Spring_Boot\spring-1.5.3.RELEASE\bin&gt;spring.bat --version
+Spring CLI v1.5.3.RELEASE</t>
+  </si>
+  <si>
+    <t>list of spring sample projects in github</t>
+  </si>
+  <si>
+    <t>https://github.com/spring-projects</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Configuration:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tags the class as a source of bean definitions for the application context.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@EnableAutoConfiguration:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tells Spring Boot to start adding beans based on classpath settings, other beans, and various property settings.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@EnableWebMvc:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Normally you would add @EnableWebMvc for a Spring MVC app, but Spring Boot adds it automatically when it sees spring-webmvc on the classpath. This flags the application as a web application and activates key behaviors such as setting up a DispatcherServlet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@ComponentScan:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tells Spring to look for other components, configurations, and services in the packages specified in basePackages attribute, allowing it to find the controllers.
+Look for all spring components (controllers, services, repositories) starting in the package of App.java and recursively looking through all sub packages from there. So make a note if we place main app class in an nested subfolder below other app folders, then ComponentScan won't be able to find the spring components. It's the best to keep the main class at the top level of main package structure. </t>
+    </r>
+  </si>
+  <si>
+    <t>1. src/main/resources -&gt; public folder
+2. src/main/resources -&gt; static folder
+3. src/main/resources folder</t>
   </si>
 </sst>
 </file>
@@ -5954,7 +6032,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -6219,6 +6297,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6256,15 +6340,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6273,12 +6354,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6578,7 +6663,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6593,7 +6678,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -6630,7 +6715,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="17"/>
@@ -6685,7 +6770,7 @@
         <v>305</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -6701,7 +6786,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>336</v>
@@ -6709,59 +6794,59 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="19" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B18" s="12"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="12" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="67" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="67" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="67" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="19" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" s="19" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="B27" s="19" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="B28" s="19" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="67" t="s">
-        <v>857</v>
+      <c r="A29" s="114" t="s">
+        <v>854</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -6782,6 +6867,7 @@
     <hyperlink ref="C1" location="Topics!A2" display="Up"/>
     <hyperlink ref="B1" location="Materials!A1" display="Materials"/>
     <hyperlink ref="A20" location="Cloud!A1" display="Spring Cloud"/>
+    <hyperlink ref="A29" location="'Data+REST'!A1" display="Spring Data REST"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6856,9 +6942,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:A16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6876,13 +6962,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="93"/>
+      <c r="B4" s="95"/>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="103" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -6890,7 +6976,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="102"/>
+      <c r="A6" s="104"/>
       <c r="B6" s="5" t="s">
         <v>108</v>
       </c>
@@ -6936,7 +7022,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="112" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -6944,7 +7030,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="110"/>
+      <c r="A13" s="112"/>
       <c r="B13" s="5" t="s">
         <v>120</v>
       </c>
@@ -6958,7 +7044,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="112" t="s">
         <v>123</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -6966,7 +7052,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="110"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="5" t="s">
         <v>125</v>
       </c>
@@ -6981,10 +7067,10 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="82" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -7004,11 +7090,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7026,24 +7112,24 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="92" t="s">
-        <v>410</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="94" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="93"/>
+      <c r="B6" s="95"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="29" t="s">
@@ -7082,7 +7168,7 @@
         <v>358</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -7109,416 +7195,479 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="30">
       <c r="A15" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>370</v>
+      <c r="B15" s="92" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45">
       <c r="A16" s="32" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="19" customFormat="1" ht="90">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="19" customFormat="1" ht="135">
       <c r="A17" s="87" t="s">
-        <v>871</v>
-      </c>
-      <c r="B17" s="87" t="s">
-        <v>872</v>
+        <v>868</v>
+      </c>
+      <c r="B17" s="92" t="s">
+        <v>910</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="29" t="s">
-        <v>372</v>
-      </c>
-      <c r="B18" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45">
+      <c r="A19" s="29" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="29" t="s">
-        <v>375</v>
-      </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="93" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45">
+      <c r="A20" s="106" t="s">
+        <v>378</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30">
+      <c r="A21" s="106"/>
+      <c r="B21" s="29" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="105" t="s">
-        <v>381</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="105"/>
-      <c r="B21" s="29" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
       <c r="A22" s="29" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
       <c r="A23" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B23" s="29" t="s">
         <v>382</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="29" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="29" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="75">
       <c r="A26" s="29" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
       <c r="A27" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="107" t="s">
         <v>389</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B28" s="29" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="120">
+      <c r="A29" s="107"/>
+      <c r="B29" s="29" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="104" t="s">
-        <v>392</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="120">
-      <c r="A29" s="104"/>
-      <c r="B29" s="29" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30">
       <c r="A30" s="29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="29" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
       <c r="A32" s="29" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60">
       <c r="A33" s="30" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="105">
       <c r="A34" s="54" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B34" s="88" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90">
       <c r="A35" s="30" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="225">
       <c r="A36" s="32" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
       <c r="A37" s="32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B37" s="54" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="32" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B38" s="54" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="32" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B39" s="54" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="19" customFormat="1">
       <c r="A40" s="45" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="105">
       <c r="A41" s="45" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="45">
-      <c r="A42" s="104" t="s">
-        <v>506</v>
+      <c r="A42" s="107" t="s">
+        <v>503</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="210">
-      <c r="A43" s="104"/>
+      <c r="A43" s="107"/>
       <c r="B43" s="48" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45">
       <c r="A44" s="49" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="B45" s="49" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30">
+      <c r="A46" s="105" t="s">
+        <v>508</v>
+      </c>
+      <c r="B46" s="49" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="49" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="120">
+      <c r="A47" s="105"/>
+      <c r="B47" s="49" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="105"/>
+      <c r="B48" s="24" t="s">
         <v>510</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="103" t="s">
-        <v>511</v>
-      </c>
-      <c r="B46" s="49" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="120">
-      <c r="A47" s="103"/>
-      <c r="B47" s="49" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="103"/>
-      <c r="B48" s="24" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="60">
       <c r="A49" s="50" t="s">
+        <v>512</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45" customHeight="1">
+      <c r="A50" s="105" t="s">
+        <v>513</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30">
+      <c r="A51" s="105"/>
+      <c r="B51" s="50" t="s">
         <v>515</v>
-      </c>
-      <c r="B49" s="53" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="45" customHeight="1">
-      <c r="A50" s="103" t="s">
-        <v>516</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="30">
-      <c r="A51" s="103"/>
-      <c r="B51" s="50" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30">
       <c r="A52" s="50" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="19" customFormat="1" ht="30">
       <c r="A53" s="50" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="45">
       <c r="A54" s="50" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
       <c r="A55" s="50" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="103" t="s">
-        <v>523</v>
+      <c r="A56" s="105" t="s">
+        <v>520</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="103"/>
+      <c r="A57" s="105"/>
       <c r="B57" s="50" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="50" t="s">
+        <v>527</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="45">
+      <c r="A59" s="111" t="s">
+        <v>529</v>
+      </c>
+      <c r="B59" s="52" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="111"/>
+      <c r="B60" s="51" t="s">
         <v>530</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="45">
-      <c r="A59" s="107" t="s">
-        <v>532</v>
-      </c>
-      <c r="B59" s="52" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="107"/>
-      <c r="B60" s="51" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30">
       <c r="A61" s="52" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B61" s="52" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="52" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B62" s="52" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="60">
       <c r="A63" s="65" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B63" s="65" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90">
       <c r="A64" s="65" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B64" s="65" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="86" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="B65" s="86" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="86" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="B66" s="86" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="75">
       <c r="A67" s="87" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B67" s="87" t="s">
-        <v>863</v>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="92" t="s">
+        <v>895</v>
+      </c>
+      <c r="B68" s="92" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="92" t="s">
+        <v>897</v>
+      </c>
+      <c r="B69" s="92" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="30">
+      <c r="A70" s="92" t="s">
+        <v>899</v>
+      </c>
+      <c r="B70" s="92" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30">
+      <c r="A71" s="92" t="s">
+        <v>901</v>
+      </c>
+      <c r="B71" s="92" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="19" customFormat="1" ht="75">
+      <c r="A72" s="106" t="s">
+        <v>905</v>
+      </c>
+      <c r="B72" s="92" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="19" customFormat="1" ht="30">
+      <c r="A73" s="106"/>
+      <c r="B73" s="92" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="60">
+      <c r="A74" s="92" t="s">
+        <v>903</v>
+      </c>
+      <c r="B74" s="92" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="92" t="s">
+        <v>908</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>909</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A72:A73"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A56:A57"/>
@@ -7537,9 +7686,10 @@
     <hyperlink ref="B40" r:id="rId3"/>
     <hyperlink ref="B48" r:id="rId4"/>
     <hyperlink ref="B52" r:id="rId5" location="auto-configuration-classes"/>
+    <hyperlink ref="B75" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -7567,10 +7717,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="94" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
@@ -7581,10 +7731,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="B6" s="93"/>
+      <c r="B6" s="95"/>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="9" t="s">
@@ -7619,7 +7769,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="105" t="s">
         <v>318</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -7627,7 +7777,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="103"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="26" t="s">
         <v>320</v>
       </c>
@@ -7641,7 +7791,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="106" t="s">
         <v>328</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -7649,13 +7799,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="105"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="26" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="105"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="26" t="s">
         <v>344</v>
       </c>
@@ -7739,8 +7889,8 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7758,149 +7908,149 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="92" t="s">
-        <v>410</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="56" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="93"/>
+      <c r="B7" s="95"/>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="56" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="56" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75">
       <c r="A10" s="56" t="s">
+        <v>558</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1">
+      <c r="A11" s="111" t="s">
+        <v>560</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>561</v>
       </c>
-      <c r="B10" s="56" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="111"/>
+      <c r="B12" s="19" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" customHeight="1">
-      <c r="A11" s="107" t="s">
-        <v>563</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="107"/>
-      <c r="B12" s="19" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="56" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30">
       <c r="A14" s="57" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="57" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75">
       <c r="A16" s="58" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60">
       <c r="A17" s="59" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75">
       <c r="A18" s="59" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="59" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="59" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
       <c r="A21" s="60" t="s">
+        <v>579</v>
+      </c>
+      <c r="B21" s="60" t="s">
         <v>582</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="105">
       <c r="A22" s="60" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="63" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -7944,93 +8094,93 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="92" t="s">
-        <v>410</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="93"/>
+      <c r="B7" s="95"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="19" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="19" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="19" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="75">
       <c r="A11" s="19" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45">
       <c r="A12" s="19" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105">
       <c r="A13" s="19" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120">
       <c r="A14" s="19" t="s">
+        <v>606</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="75">
+      <c r="A15" s="113" t="s">
+        <v>608</v>
+      </c>
+      <c r="B15" s="66" t="s">
         <v>609</v>
       </c>
-      <c r="B14" s="66" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="30">
+      <c r="A16" s="113"/>
+      <c r="B16" s="66" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="111" t="s">
-        <v>611</v>
-      </c>
-      <c r="B15" s="66" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="111"/>
-      <c r="B16" s="66" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75">
       <c r="A17" s="67" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -8049,11 +8199,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8063,125 +8213,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="19" t="s">
-        <v>865</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>866</v>
-      </c>
+    <row r="2" spans="1:2" s="19" customFormat="1">
+      <c r="A2" s="94" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="19" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="19" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="19" t="s">
-        <v>873</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>874</v>
+        <v>866</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="19" t="s">
-        <v>875</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="75">
+        <v>869</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="19" t="s">
-        <v>877</v>
-      </c>
-      <c r="B7" s="87" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>871</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="75">
       <c r="A8" s="19" t="s">
-        <v>879</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>880</v>
+        <v>873</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="19" t="s">
+        <v>875</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="19" t="s">
+        <v>877</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="19" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30">
+      <c r="A12" s="19" t="s">
+        <v>880</v>
+      </c>
+      <c r="B12" s="87" t="s">
         <v>881</v>
       </c>
-      <c r="B9" s="19" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="45">
+      <c r="A13" s="19" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" s="19" t="s">
+      <c r="B13" s="87" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30">
-      <c r="A11" s="19" t="s">
-        <v>884</v>
-      </c>
-      <c r="B11" s="87" t="s">
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="19" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="45">
-      <c r="A12" s="19" t="s">
+      <c r="B14" s="89" t="s">
         <v>886</v>
       </c>
-      <c r="B12" s="87" t="s">
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="19" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="30">
-      <c r="A13" s="19" t="s">
+      <c r="B15" s="89" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="120">
+      <c r="A16" s="19" t="s">
         <v>889</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B16" s="89" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="19" t="s">
-        <v>891</v>
-      </c>
-      <c r="B14" s="89" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="120">
-      <c r="A15" s="19" t="s">
-        <v>893</v>
-      </c>
-      <c r="B15" s="89" t="s">
-        <v>894</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B1" location="'Data+REST'!A2" display="Up"/>
+    <hyperlink ref="A1" location="Topics!A29" display="Topics"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8211,29 +8372,29 @@
         <v>11</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="19" customFormat="1">
-      <c r="A2" s="92" t="s">
-        <v>485</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="19" customFormat="1"/>
     <row r="5" spans="1:3">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="94" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="93"/>
+      <c r="B5" s="95"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="29" t="s">
@@ -8243,7 +8404,7 @@
         <v>362</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8251,36 +8412,36 @@
         <v>361</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="95"/>
+      <c r="B9" s="97"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="19" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="93"/>
+      <c r="B12" s="95"/>
     </row>
     <row r="13" spans="1:3" s="19" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -8317,33 +8478,33 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="19" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="94" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="95"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="19" t="s">
@@ -8389,32 +8550,32 @@
       <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="92" t="s">
-        <v>639</v>
-      </c>
-      <c r="B29" s="93"/>
+      <c r="A29" s="94" t="s">
+        <v>636</v>
+      </c>
+      <c r="B29" s="95"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="67" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="19" customFormat="1"/>
     <row r="32" spans="1:2">
-      <c r="A32" s="92" t="s">
-        <v>550</v>
-      </c>
-      <c r="B32" s="93"/>
+      <c r="A32" s="94" t="s">
+        <v>547</v>
+      </c>
+      <c r="B32" s="95"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
         <v>363</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -8422,7 +8583,7 @@
         <v>363</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -8430,45 +8591,45 @@
       <c r="B35" s="19"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="93"/>
+      <c r="B37" s="95"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="19" t="s">
         <v>363</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="92" t="s">
-        <v>586</v>
-      </c>
-      <c r="B40" s="93"/>
+      <c r="A40" s="94" t="s">
+        <v>583</v>
+      </c>
+      <c r="B40" s="95"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="19" t="s">
         <v>363</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="97"/>
+      <c r="B43" s="99"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="19" t="s">
         <v>361</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -8531,42 +8692,42 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="94" t="s">
-        <v>661</v>
-      </c>
-      <c r="B2" s="95"/>
+      <c r="A2" s="96" t="s">
+        <v>658</v>
+      </c>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="19" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1">
       <c r="A4" s="19" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="19" customFormat="1"/>
     <row r="6" spans="1:2" s="19" customFormat="1"/>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="94" t="s">
-        <v>662</v>
-      </c>
-      <c r="B8" s="95"/>
+      <c r="A8" s="96" t="s">
+        <v>659</v>
+      </c>
+      <c r="B8" s="97"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="19" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1"/>
@@ -8578,13 +8739,13 @@
     <row r="16" spans="1:2" s="19" customFormat="1"/>
     <row r="17" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="18" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="95"/>
+      <c r="B18" s="97"/>
     </row>
     <row r="19" spans="1:2" ht="45">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="103" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -8592,7 +8753,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="102"/>
+      <c r="A20" s="104"/>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
@@ -8602,7 +8763,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60">
@@ -8818,7 +8979,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30">
@@ -8870,7 +9031,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="45">
-      <c r="A55" s="102" t="s">
+      <c r="A55" s="104" t="s">
         <v>81</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -8878,19 +9039,19 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="45">
-      <c r="A56" s="102"/>
+      <c r="A56" s="104"/>
       <c r="B56" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="102"/>
+      <c r="A57" s="104"/>
       <c r="B57" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="102" t="s">
+      <c r="A58" s="104" t="s">
         <v>85</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -8898,19 +9059,19 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
-      <c r="A59" s="102"/>
+      <c r="A59" s="104"/>
       <c r="B59" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90">
-      <c r="A60" s="102"/>
+      <c r="A60" s="104"/>
       <c r="B60" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="75">
-      <c r="A61" s="102" t="s">
+      <c r="A61" s="104" t="s">
         <v>89</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -8918,7 +9079,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="45">
-      <c r="A62" s="102"/>
+      <c r="A62" s="104"/>
       <c r="B62" s="5" t="s">
         <v>322</v>
       </c>
@@ -8972,7 +9133,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
-      <c r="A69" s="100" t="s">
+      <c r="A69" s="102" t="s">
         <v>102</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -8980,20 +9141,20 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="240">
-      <c r="A70" s="100"/>
+      <c r="A70" s="102"/>
       <c r="B70" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="180">
-      <c r="A71" s="100"/>
+      <c r="A71" s="102"/>
       <c r="B71" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30">
       <c r="A72" s="46" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>304</v>
@@ -9017,138 +9178,138 @@
     </row>
     <row r="75" spans="1:2" ht="60">
       <c r="A75" s="31" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30">
       <c r="A76" s="34" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B76" s="35" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="19" customFormat="1" ht="30">
       <c r="A77" s="79" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="B77" s="80" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105">
-      <c r="A78" s="99" t="s">
-        <v>464</v>
+      <c r="A78" s="101" t="s">
+        <v>461</v>
       </c>
       <c r="B78" s="35" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="120">
-      <c r="A79" s="99"/>
+      <c r="A79" s="101"/>
       <c r="B79" s="35" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="75">
+      <c r="A80" s="101"/>
+      <c r="B80" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="60">
+      <c r="A81" s="101" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="75">
-      <c r="A80" s="99"/>
-      <c r="B80" s="35" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="60">
-      <c r="A81" s="99" t="s">
-        <v>465</v>
-      </c>
       <c r="B81" s="43" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="60">
-      <c r="A82" s="99"/>
+      <c r="A82" s="101"/>
       <c r="B82" s="43" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="30">
       <c r="A83" s="37" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="60">
       <c r="A84" s="37" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="45">
       <c r="A85" s="37" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B85" s="38" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="30">
       <c r="A86" s="72" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75">
       <c r="A87" s="41" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="39" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="45">
       <c r="A89" s="39" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="98" t="s">
-        <v>490</v>
+      <c r="A90" s="100" t="s">
+        <v>487</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="98"/>
+      <c r="A91" s="100"/>
       <c r="B91" s="43" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="30">
       <c r="A92" s="90" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="B92" s="91" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -9199,10 +9360,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="93"/>
+      <c r="B4" s="95"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
@@ -9432,10 +9593,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="93"/>
+      <c r="B3" s="95"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
@@ -9447,18 +9608,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="19" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="19" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
   </sheetData>
@@ -9497,10 +9658,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="92" t="s">
-        <v>661</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="76"/>
@@ -9518,10 +9679,10 @@
       <c r="A7" s="76"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
-      <c r="A8" s="92" t="s">
-        <v>667</v>
-      </c>
-      <c r="B8" s="93"/>
+      <c r="A8" s="94" t="s">
+        <v>664</v>
+      </c>
+      <c r="B8" s="95"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="76"/>
@@ -9548,10 +9709,10 @@
       <c r="A16" s="76"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="92" t="s">
-        <v>655</v>
-      </c>
-      <c r="B18" s="93"/>
+      <c r="A18" s="94" t="s">
+        <v>652</v>
+      </c>
+      <c r="B18" s="95"/>
     </row>
     <row r="19" spans="1:2" ht="90">
       <c r="A19" s="75" t="s">
@@ -9722,63 +9883,63 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="92" t="s">
-        <v>656</v>
-      </c>
-      <c r="B41" s="93"/>
+      <c r="A41" s="94" t="s">
+        <v>653</v>
+      </c>
+      <c r="B41" s="95"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="46" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="103" t="s">
-        <v>660</v>
+      <c r="A43" s="105" t="s">
+        <v>657</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="103"/>
+      <c r="A44" s="105"/>
       <c r="B44" s="19" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90">
       <c r="A45" s="76" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B45" s="76" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="45">
       <c r="A46" s="76" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B46" s="76" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="19" customFormat="1" ht="45">
       <c r="A47" s="77" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="77" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -9786,7 +9947,7 @@
         <v>201</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
@@ -9794,538 +9955,538 @@
         <v>187</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
       <c r="A51" s="78" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B51" s="78" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="78" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B52" s="78" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="78" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B53" s="78" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="75">
       <c r="A54" s="78" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B54" s="78" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="78" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B55" s="78" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="78" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B56" s="78" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="78" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="78" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B58" s="78" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
       <c r="A59" s="78" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B59" s="78" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="60">
       <c r="A60" s="80" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B60" s="80" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="19" customFormat="1">
       <c r="A61" s="80" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B61" s="80" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="19" customFormat="1">
       <c r="A62" s="80" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="B62" s="80" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="19" customFormat="1">
       <c r="A63" s="80" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="B63" s="80" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="60">
       <c r="A64" s="80" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="B64" s="80" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="60">
       <c r="A65" s="80" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B65" s="80" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="240">
       <c r="A66" s="80" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B66" s="80" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="105">
       <c r="A67" s="80" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="B67" s="80" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="60">
       <c r="A68" s="80" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="B68" s="80" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="120">
       <c r="A69" s="80" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="B69" s="80" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="120">
+      <c r="A70" s="105" t="s">
+        <v>732</v>
+      </c>
+      <c r="B70" s="80" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120">
-      <c r="A70" s="103" t="s">
-        <v>735</v>
-      </c>
-      <c r="B70" s="80" t="s">
-        <v>736</v>
-      </c>
-    </row>
     <row r="71" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A71" s="103"/>
+      <c r="A71" s="105"/>
       <c r="B71" s="80" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60">
-      <c r="A72" s="103" t="s">
-        <v>743</v>
+      <c r="A72" s="105" t="s">
+        <v>740</v>
       </c>
       <c r="B72" s="80" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="60">
-      <c r="A73" s="103"/>
+      <c r="A73" s="105"/>
       <c r="B73" s="80" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120">
       <c r="A74" s="80" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="B74" s="83" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="60">
       <c r="A75" s="80" t="s">
+        <v>745</v>
+      </c>
+      <c r="B75" s="80" t="s">
         <v>748</v>
-      </c>
-      <c r="B75" s="80" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="80" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B76" s="80" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="60">
       <c r="A77" s="80" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B77" s="80" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="45">
       <c r="A78" s="80" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="B78" s="80" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="45">
       <c r="A79" s="80" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B79" s="80" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="80" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="B80" s="80" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="75">
       <c r="A81" s="80" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="B81" s="80" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="75">
       <c r="A82" s="80" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B82" s="80" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75">
       <c r="A83" s="80" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B83" s="80" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90">
       <c r="A84" s="80" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B84" s="80" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="80" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="B85" s="80" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="80" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B86" s="80" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30">
       <c r="A87" s="80" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="B87" s="80" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30">
       <c r="A88" s="80" t="s">
+        <v>771</v>
+      </c>
+      <c r="B88" s="80" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="105" t="s">
+        <v>773</v>
+      </c>
+      <c r="B89" s="83" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="90">
+      <c r="A90" s="105"/>
+      <c r="B90" s="80" t="s">
         <v>774</v>
       </c>
-      <c r="B88" s="80" t="s">
+    </row>
+    <row r="91" spans="1:2" ht="75">
+      <c r="A91" s="105"/>
+      <c r="B91" s="80" t="s">
         <v>775</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="103" t="s">
-        <v>776</v>
-      </c>
-      <c r="B89" s="83" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="90">
-      <c r="A90" s="103"/>
-      <c r="B90" s="80" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="75">
-      <c r="A91" s="103"/>
-      <c r="B91" s="80" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="30">
       <c r="A92" s="80" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B92" s="80" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="30">
       <c r="A93" s="80" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="B93" s="80" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="120">
       <c r="A94" s="80" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B94" s="80" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="80" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="B95" s="80" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="30">
       <c r="A96" s="80" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B96" s="81" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="80" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="B97" s="80" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="30">
       <c r="A98" s="80" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="B98" s="80" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30">
       <c r="A99" s="80" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B99" s="81" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="30">
       <c r="A100" s="80" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B100" s="81" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="80" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="B101" s="80" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120">
       <c r="A102" s="81" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B102" s="81" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="30">
       <c r="A103" s="81" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="B103" s="81" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90">
       <c r="A104" s="81" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B104" s="81" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90">
       <c r="A105" s="81" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B105" s="81" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="60">
       <c r="A106" s="81" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B106" s="81" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="81" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="81" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B108" s="81" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="75">
       <c r="A109" s="81" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="B109" s="81" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="81" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="B110" s="81" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="60">
+      <c r="A111" s="105" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" ht="60">
-      <c r="A111" s="103" t="s">
-        <v>817</v>
-      </c>
       <c r="B111" s="81" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="60">
-      <c r="A112" s="103"/>
+      <c r="A112" s="105"/>
       <c r="B112" s="81" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="60">
       <c r="A113" s="81" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="B113" s="81" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="114" spans="1:2" s="19" customFormat="1" ht="60">
       <c r="A114" s="81" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="B114" s="81" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="45">
       <c r="A115" s="81" t="s">
+        <v>817</v>
+      </c>
+      <c r="B115" s="81" t="s">
         <v>820</v>
-      </c>
-      <c r="B115" s="81" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120">
       <c r="A116" s="81" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B116" s="81" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="75">
       <c r="A117" s="81" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="B117" s="81" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="225">
       <c r="A118" s="81" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B118" s="81" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
@@ -10376,17 +10537,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="92" t="s">
-        <v>646</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>643</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="6" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1">
@@ -10402,10 +10563,10 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1">
-      <c r="A7" s="92" t="s">
-        <v>647</v>
-      </c>
-      <c r="B7" s="93"/>
+      <c r="A7" s="94" t="s">
+        <v>644</v>
+      </c>
+      <c r="B7" s="95"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
       <c r="A8" s="6"/>
@@ -10428,10 +10589,10 @@
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="95"/>
     </row>
     <row r="14" spans="1:2" ht="75">
       <c r="A14" s="33" t="s">
@@ -10442,7 +10603,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="120">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="104" t="s">
         <v>301</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -10450,13 +10611,13 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="240">
-      <c r="A16" s="102"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="101" t="s">
         <v>316</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -10464,301 +10625,295 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="120">
-      <c r="A18" s="99"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="68" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135">
-      <c r="A19" s="99"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="84" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="150">
-      <c r="A20" s="105" t="s">
-        <v>433</v>
+      <c r="A20" s="106" t="s">
+        <v>430</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A21" s="105"/>
+      <c r="A21" s="106"/>
       <c r="B21" s="33" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="106" t="s">
+        <v>408</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="60">
+      <c r="A23" s="106"/>
+      <c r="B23" s="61" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="45">
+      <c r="A24" s="106"/>
+      <c r="B24" s="33" t="s">
         <v>411</v>
       </c>
-      <c r="B22" s="33" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="30">
+      <c r="A25" s="106" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="60">
-      <c r="A23" s="105"/>
-      <c r="B23" s="61" t="s">
+      <c r="B25" s="33" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="105"/>
-      <c r="B24" s="33" t="s">
+    <row r="26" spans="1:2" ht="135">
+      <c r="A26" s="106"/>
+      <c r="B26" s="33" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30">
-      <c r="A25" s="105" t="s">
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="106"/>
+      <c r="B27" s="33" t="s">
         <v>415</v>
       </c>
-      <c r="B25" s="33" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="45">
+      <c r="A28" s="106"/>
+      <c r="B28" s="33" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="135">
-      <c r="A26" s="105"/>
-      <c r="B26" s="33" t="s">
+    <row r="29" spans="1:2" ht="30">
+      <c r="A29" s="106"/>
+      <c r="B29" s="33" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="105"/>
-      <c r="B27" s="33" t="s">
+    <row r="30" spans="1:2" ht="45">
+      <c r="A30" s="107" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="105"/>
-      <c r="B28" s="33" t="s">
+      <c r="B30" s="33" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="105"/>
-      <c r="B29" s="33" t="s">
+    <row r="31" spans="1:2" ht="45">
+      <c r="A31" s="107"/>
+      <c r="B31" s="33" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="104" t="s">
+    <row r="32" spans="1:2" ht="30">
+      <c r="A32" s="107"/>
+      <c r="B32" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="B30" s="33" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="45">
+      <c r="A33" s="107"/>
+      <c r="B33" s="33" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="104"/>
-      <c r="B31" s="33" t="s">
+    <row r="34" spans="1:2" ht="45">
+      <c r="A34" s="107"/>
+      <c r="B34" s="33" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="104"/>
-      <c r="B32" s="33" t="s">
+    <row r="35" spans="1:2" ht="30">
+      <c r="A35" s="106" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="104"/>
-      <c r="B33" s="33" t="s">
+      <c r="B35" s="33" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="104"/>
-      <c r="B34" s="33" t="s">
+    <row r="36" spans="1:2" ht="165">
+      <c r="A36" s="106"/>
+      <c r="B36" s="33" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30">
-      <c r="A35" s="105" t="s">
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="106"/>
+      <c r="B37" s="33" t="s">
         <v>427</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="165">
-      <c r="A36" s="105"/>
-      <c r="B36" s="33" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="105"/>
-      <c r="B37" s="33" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30">
       <c r="A38" s="47" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="60">
       <c r="A39" s="33" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="60">
       <c r="A40" s="33" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75">
       <c r="A41" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30">
+      <c r="A42" s="106" t="s">
+        <v>438</v>
+      </c>
+      <c r="B42" s="33" t="s">
         <v>439</v>
       </c>
-      <c r="B41" s="33" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="75">
+      <c r="A43" s="106"/>
+      <c r="B43" s="33" t="s">
         <v>440</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="30">
-      <c r="A42" s="105" t="s">
-        <v>441</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="75">
-      <c r="A43" s="105"/>
-      <c r="B43" s="33" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120">
       <c r="A44" s="33" t="s">
+        <v>441</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30">
+      <c r="A45" s="106" t="s">
+        <v>443</v>
+      </c>
+      <c r="B45" s="33" t="s">
         <v>444</v>
       </c>
-      <c r="B44" s="33" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="30">
+      <c r="A46" s="106"/>
+      <c r="B46" s="33" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="105" t="s">
-        <v>446</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="105"/>
-      <c r="B46" s="33" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="135">
       <c r="A47" s="33" t="s">
+        <v>446</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30">
+      <c r="A48" s="106" t="s">
+        <v>443</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="60">
+      <c r="A49" s="106"/>
+      <c r="B49" s="33" t="s">
         <v>449</v>
       </c>
-      <c r="B47" s="33" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="30">
-      <c r="A48" s="105" t="s">
-        <v>446</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="60">
-      <c r="A49" s="105"/>
-      <c r="B49" s="33" t="s">
-        <v>452</v>
-      </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="104" t="s">
-        <v>588</v>
+      <c r="A50" s="107" t="s">
+        <v>585</v>
       </c>
       <c r="B50" s="62" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="60">
-      <c r="A51" s="104"/>
+      <c r="A51" s="107"/>
       <c r="B51" s="62" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="92" t="s">
-        <v>836</v>
-      </c>
-      <c r="B53" s="93"/>
+      <c r="A53" s="94" t="s">
+        <v>833</v>
+      </c>
+      <c r="B53" s="95"/>
     </row>
     <row r="54" spans="1:2" ht="45">
       <c r="A54" s="84" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B54" s="84" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
       <c r="A55" s="84" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="B55" s="84" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45">
       <c r="A56" s="84" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="B56" s="84" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
       <c r="A57" s="85" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B57" s="85" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
       <c r="A58" s="85" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B58" s="85" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90">
       <c r="A59" s="85" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="B59" s="85" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A48:A49"/>
@@ -10768,6 +10923,12 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -10802,10 +10963,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="93"/>
+      <c r="B3" s="95"/>
     </row>
     <row r="4" spans="1:2" ht="60">
       <c r="A4" s="6" t="s">
@@ -10856,7 +11017,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="104" t="s">
         <v>242</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -10864,25 +11025,25 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="102"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="5" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="102"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="5" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="108" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="106"/>
+      <c r="B13" s="108"/>
     </row>
     <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="104" t="s">
         <v>247</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -10890,13 +11051,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="102"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
-      <c r="A16" s="102"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="5" t="s">
         <v>250</v>
       </c>
@@ -10926,7 +11087,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="102" t="s">
+      <c r="A20" s="104" t="s">
         <v>257</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -10934,7 +11095,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="102"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="5" t="s">
         <v>259</v>
       </c>
@@ -11012,7 +11173,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="102" t="s">
+      <c r="A31" s="104" t="s">
         <v>278</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -11020,13 +11181,13 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="102"/>
+      <c r="A32" s="104"/>
       <c r="B32" s="5" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="102"/>
+      <c r="A33" s="104"/>
       <c r="B33" s="5" t="s">
         <v>281</v>
       </c>
@@ -11080,10 +11241,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="92" t="s">
-        <v>646</v>
-      </c>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94" t="s">
+        <v>643</v>
+      </c>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1"/>
     <row r="5" spans="1:2">
@@ -11100,37 +11261,37 @@
       <c r="A9" s="69"/>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="94" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="95"/>
+    </row>
+    <row r="11" spans="1:2" s="19" customFormat="1">
+      <c r="A11" s="110" t="s">
+        <v>651</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="19" customFormat="1">
+      <c r="A12" s="111"/>
+      <c r="B12" s="12" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="19" customFormat="1">
+      <c r="A13" s="111" t="s">
         <v>650</v>
       </c>
-      <c r="B10" s="93"/>
-    </row>
-    <row r="11" spans="1:2" s="19" customFormat="1">
-      <c r="A11" s="109" t="s">
-        <v>654</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="19" customFormat="1">
-      <c r="A12" s="107"/>
-      <c r="B12" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="19" customFormat="1">
-      <c r="A13" s="107" t="s">
-        <v>653</v>
-      </c>
       <c r="B13" s="19" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="19" customFormat="1">
-      <c r="A14" s="107"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="12" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="19" customFormat="1">
@@ -11155,10 +11316,10 @@
       <c r="A21" s="69"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="94" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="95"/>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1">
       <c r="A23" s="69" t="s">
@@ -11170,10 +11331,10 @@
     </row>
     <row r="24" spans="1:2" s="19" customFormat="1" ht="45">
       <c r="A24" s="69" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -11186,189 +11347,189 @@
     </row>
     <row r="26" spans="1:2" ht="30">
       <c r="A26" s="69" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="69" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B27" s="68" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
       <c r="A28" s="69" t="s">
+        <v>620</v>
+      </c>
+      <c r="B28" s="68" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="60">
+      <c r="A29" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="68" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="165">
+      <c r="A30" s="107"/>
+      <c r="B30" s="68" t="s">
         <v>623</v>
       </c>
-      <c r="B28" s="68" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="45">
+      <c r="A31" s="109" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="60">
-      <c r="A29" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="68" t="s">
+      <c r="B31" s="68" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="165">
-      <c r="A30" s="104"/>
-      <c r="B30" s="68" t="s">
+    <row r="32" spans="1:2" ht="45">
+      <c r="A32" s="109"/>
+      <c r="B32" s="68" t="s">
         <v>626</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="108" t="s">
-        <v>627</v>
-      </c>
-      <c r="B31" s="68" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="45">
-      <c r="A32" s="108"/>
-      <c r="B32" s="68" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="19" customFormat="1" ht="75">
       <c r="A33" s="70" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B33" s="68" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="60">
       <c r="A34" s="71" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B34" s="68" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="105">
       <c r="A35" s="71" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B35" s="68" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="150">
       <c r="A36" s="73" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="19" customFormat="1" ht="30">
       <c r="A37" s="73" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="B37" s="73" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="19" customFormat="1" ht="30">
       <c r="A38" s="73" t="s">
+        <v>671</v>
+      </c>
+      <c r="B38" s="73" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="90">
+      <c r="A39" s="111" t="s">
+        <v>672</v>
+      </c>
+      <c r="B39" s="73" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="120">
+      <c r="A40" s="111"/>
+      <c r="B40" s="73" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="19" customFormat="1" ht="60">
+      <c r="A41" s="105" t="s">
+        <v>676</v>
+      </c>
+      <c r="B41" s="73" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="19" customFormat="1" ht="105">
+      <c r="A42" s="105"/>
+      <c r="B42" s="73" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="105" t="s">
+        <v>673</v>
+      </c>
+      <c r="B43" s="73" t="s">
         <v>674</v>
       </c>
-      <c r="B38" s="73" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="30">
+      <c r="A44" s="105"/>
+      <c r="B44" s="73" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="75">
+      <c r="A45" s="105" t="s">
+        <v>682</v>
+      </c>
+      <c r="B45" s="73" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="107" t="s">
-        <v>675</v>
-      </c>
-      <c r="B39" s="73" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="120">
-      <c r="A40" s="107"/>
-      <c r="B40" s="73" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A41" s="103" t="s">
-        <v>679</v>
-      </c>
-      <c r="B41" s="73" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A42" s="103"/>
-      <c r="B42" s="73" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="103" t="s">
-        <v>676</v>
-      </c>
-      <c r="B43" s="73" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="103"/>
-      <c r="B44" s="73" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="75">
-      <c r="A45" s="103" t="s">
-        <v>685</v>
-      </c>
-      <c r="B45" s="73" t="s">
-        <v>686</v>
-      </c>
-    </row>
     <row r="46" spans="1:2" ht="60">
-      <c r="A46" s="103"/>
+      <c r="A46" s="105"/>
       <c r="B46" s="73" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105">
       <c r="A47" s="73" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="120">
       <c r="A48" s="73" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B48" s="73" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>

<commit_message>
spring, cloud computing, jvm, todo
spring, cloud computing, jvm, todo
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -5676,11 +5676,6 @@
     <t>Create spring boot project using spring boot cli</t>
   </si>
   <si>
-    <t>E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects&gt;E:\Backup\JavaPrep\Spring\Spring_Boot\spring-1.5.3.RELEASE\bin\spring.bat init --dependencies=web mySpringBootAppFromCLI
-Using service at https://start.spring.io
-Project extracted to 'E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects\mySpringBootAppFromCLI'</t>
-  </si>
-  <si>
     <t>Installing Spring Boot CLI</t>
   </si>
   <si>
@@ -5819,6 +5814,12 @@
     <t>1. src/main/resources -&gt; public folder
 2. src/main/resources -&gt; static folder
 3. src/main/resources folder</t>
+  </si>
+  <si>
+    <t>E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects&gt;
+E:\Backup\JavaPrep\Spring\Spring_Boot\spring-1.5.3.RELEASE\bin\spring.bat init --dependencies=web mySpringBootAppFromCLI
+Using service at https://start.spring.io
+Project extracted to 'E:\Backup\JavaPrep\practiceProjects\Spring\SpringBootProjects\mySpringBootAppFromCLI'</t>
   </si>
 </sst>
 </file>
@@ -6032,7 +6033,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -6303,6 +6304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6340,12 +6345,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6354,16 +6362,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6842,7 +6846,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="114" t="s">
+      <c r="A29" s="95" t="s">
         <v>854</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -6962,13 +6966,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="97"/>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="105" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -6976,7 +6980,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="104"/>
+      <c r="A6" s="106"/>
       <c r="B6" s="5" t="s">
         <v>108</v>
       </c>
@@ -7022,7 +7026,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="114" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -7030,7 +7034,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="112"/>
+      <c r="A13" s="114"/>
       <c r="B13" s="5" t="s">
         <v>120</v>
       </c>
@@ -7044,7 +7048,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="112" t="s">
+      <c r="A15" s="114" t="s">
         <v>123</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -7052,7 +7056,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="112"/>
+      <c r="A16" s="114"/>
       <c r="B16" s="5" t="s">
         <v>125</v>
       </c>
@@ -7093,8 +7097,8 @@
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7112,10 +7116,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="29" t="s">
@@ -7126,10 +7130,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="97"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="29" t="s">
@@ -7216,7 +7220,7 @@
         <v>868</v>
       </c>
       <c r="B17" s="92" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -7232,11 +7236,11 @@
         <v>373</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="106" t="s">
+      <c r="A20" s="109" t="s">
         <v>378</v>
       </c>
       <c r="B20" s="54" t="s">
@@ -7244,7 +7248,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="106"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="29" t="s">
         <v>376</v>
       </c>
@@ -7298,7 +7302,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="108" t="s">
         <v>389</v>
       </c>
       <c r="B28" s="29" t="s">
@@ -7306,7 +7310,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="120">
-      <c r="A29" s="107"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="29" t="s">
         <v>390</v>
       </c>
@@ -7408,7 +7412,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="45">
-      <c r="A42" s="107" t="s">
+      <c r="A42" s="108" t="s">
         <v>503</v>
       </c>
       <c r="B42" s="48" t="s">
@@ -7416,7 +7420,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="210">
-      <c r="A43" s="107"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="48" t="s">
         <v>502</v>
       </c>
@@ -7438,7 +7442,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="105" t="s">
+      <c r="A46" s="107" t="s">
         <v>508</v>
       </c>
       <c r="B46" s="49" t="s">
@@ -7446,13 +7450,13 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="120">
-      <c r="A47" s="105"/>
+      <c r="A47" s="107"/>
       <c r="B47" s="49" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="105"/>
+      <c r="A48" s="107"/>
       <c r="B48" s="24" t="s">
         <v>510</v>
       </c>
@@ -7466,7 +7470,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="45" customHeight="1">
-      <c r="A50" s="105" t="s">
+      <c r="A50" s="107" t="s">
         <v>513</v>
       </c>
       <c r="B50" s="50" t="s">
@@ -7474,7 +7478,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
-      <c r="A51" s="105"/>
+      <c r="A51" s="107"/>
       <c r="B51" s="50" t="s">
         <v>515</v>
       </c>
@@ -7512,7 +7516,7 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="107" t="s">
         <v>520</v>
       </c>
       <c r="B56" s="50" t="s">
@@ -7520,7 +7524,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="105"/>
+      <c r="A57" s="107"/>
       <c r="B57" s="50" t="s">
         <v>526</v>
       </c>
@@ -7636,47 +7640,47 @@
       </c>
     </row>
     <row r="72" spans="1:2" s="19" customFormat="1" ht="75">
-      <c r="A72" s="106" t="s">
+      <c r="A72" s="109" t="s">
+        <v>904</v>
+      </c>
+      <c r="B72" s="94" t="s">
         <v>905</v>
       </c>
-      <c r="B72" s="92" t="s">
+    </row>
+    <row r="73" spans="1:2" s="19" customFormat="1" ht="30">
+      <c r="A73" s="109"/>
+      <c r="B73" s="94" t="s">
         <v>906</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" s="19" customFormat="1" ht="30">
-      <c r="A73" s="106"/>
-      <c r="B73" s="92" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60">
       <c r="A74" s="92" t="s">
         <v>903</v>
       </c>
-      <c r="B74" s="92" t="s">
-        <v>904</v>
+      <c r="B74" s="94" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="92" t="s">
+        <v>907</v>
+      </c>
+      <c r="B75" s="24" t="s">
         <v>908</v>
-      </c>
-      <c r="B75" s="24" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A72:A73"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A56:A57"/>
     <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Boot!A2" display="Up"/>
@@ -7717,10 +7721,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
@@ -7731,10 +7735,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="97"/>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" s="9" t="s">
@@ -7769,7 +7773,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="107" t="s">
         <v>318</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -7777,7 +7781,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="105"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="26" t="s">
         <v>320</v>
       </c>
@@ -7791,7 +7795,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="109" t="s">
         <v>328</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -7799,13 +7803,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="106"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="26" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="106"/>
+      <c r="A16" s="109"/>
       <c r="B16" s="26" t="s">
         <v>344</v>
       </c>
@@ -7908,10 +7912,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="56" t="s">
@@ -7922,10 +7926,10 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="97"/>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="56" t="s">
@@ -8094,16 +8098,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="97"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="19" t="s">
@@ -8162,7 +8166,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="115" t="s">
         <v>608</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -8170,7 +8174,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="113"/>
+      <c r="A16" s="115"/>
       <c r="B16" s="66" t="s">
         <v>610</v>
       </c>
@@ -8221,10 +8225,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="19" t="s">
@@ -8376,10 +8380,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="19" customFormat="1">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>482</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
@@ -8391,10 +8395,10 @@
     </row>
     <row r="4" spans="1:3" s="19" customFormat="1"/>
     <row r="5" spans="1:3">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="96" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="95"/>
+      <c r="B5" s="97"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="29" t="s">
@@ -8417,10 +8421,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="97"/>
+      <c r="B9" s="99"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="19" t="s">
@@ -8431,10 +8435,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="95"/>
+      <c r="B12" s="97"/>
     </row>
     <row r="13" spans="1:3" s="19" customFormat="1">
       <c r="A13" s="6" t="s">
@@ -8501,10 +8505,10 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="96" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="95"/>
+      <c r="B22" s="97"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="19" t="s">
@@ -8550,10 +8554,10 @@
       <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="94" t="s">
+      <c r="A29" s="96" t="s">
         <v>636</v>
       </c>
-      <c r="B29" s="95"/>
+      <c r="B29" s="97"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="67" t="s">
@@ -8565,10 +8569,10 @@
     </row>
     <row r="31" spans="1:2" s="19" customFormat="1"/>
     <row r="32" spans="1:2">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="96" t="s">
         <v>547</v>
       </c>
-      <c r="B32" s="95"/>
+      <c r="B32" s="97"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
@@ -8591,10 +8595,10 @@
       <c r="B35" s="19"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="95"/>
+      <c r="B37" s="97"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="19" t="s">
@@ -8605,10 +8609,10 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="94" t="s">
+      <c r="A40" s="96" t="s">
         <v>583</v>
       </c>
-      <c r="B40" s="95"/>
+      <c r="B40" s="97"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="19" t="s">
@@ -8619,10 +8623,10 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="99"/>
+      <c r="B43" s="101"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="19" t="s">
@@ -8692,10 +8696,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="98" t="s">
         <v>658</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="99"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="19" t="s">
@@ -8717,10 +8721,10 @@
     <row r="6" spans="1:2" s="19" customFormat="1"/>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="98" t="s">
         <v>659</v>
       </c>
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="19" t="s">
@@ -8739,13 +8743,13 @@
     <row r="16" spans="1:2" s="19" customFormat="1"/>
     <row r="17" spans="1:2" s="19" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="18" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="97"/>
+      <c r="B18" s="99"/>
     </row>
     <row r="19" spans="1:2" ht="45">
-      <c r="A19" s="103" t="s">
+      <c r="A19" s="105" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -8753,7 +8757,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="104"/>
+      <c r="A20" s="106"/>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
@@ -9031,7 +9035,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="45">
-      <c r="A55" s="104" t="s">
+      <c r="A55" s="106" t="s">
         <v>81</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -9039,19 +9043,19 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="45">
-      <c r="A56" s="104"/>
+      <c r="A56" s="106"/>
       <c r="B56" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="104"/>
+      <c r="A57" s="106"/>
       <c r="B57" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="104" t="s">
+      <c r="A58" s="106" t="s">
         <v>85</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -9059,19 +9063,19 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="30">
-      <c r="A59" s="104"/>
+      <c r="A59" s="106"/>
       <c r="B59" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90">
-      <c r="A60" s="104"/>
+      <c r="A60" s="106"/>
       <c r="B60" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="75">
-      <c r="A61" s="104" t="s">
+      <c r="A61" s="106" t="s">
         <v>89</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -9079,7 +9083,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="45">
-      <c r="A62" s="104"/>
+      <c r="A62" s="106"/>
       <c r="B62" s="5" t="s">
         <v>322</v>
       </c>
@@ -9133,7 +9137,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
-      <c r="A69" s="102" t="s">
+      <c r="A69" s="104" t="s">
         <v>102</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -9141,13 +9145,13 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="240">
-      <c r="A70" s="102"/>
+      <c r="A70" s="104"/>
       <c r="B70" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="180">
-      <c r="A71" s="102"/>
+      <c r="A71" s="104"/>
       <c r="B71" s="5" t="s">
         <v>105</v>
       </c>
@@ -9201,7 +9205,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" ht="105">
-      <c r="A78" s="101" t="s">
+      <c r="A78" s="103" t="s">
         <v>461</v>
       </c>
       <c r="B78" s="35" t="s">
@@ -9209,19 +9213,19 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="120">
-      <c r="A79" s="101"/>
+      <c r="A79" s="103"/>
       <c r="B79" s="35" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75">
-      <c r="A80" s="101"/>
+      <c r="A80" s="103"/>
       <c r="B80" s="35" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="60">
-      <c r="A81" s="101" t="s">
+      <c r="A81" s="103" t="s">
         <v>462</v>
       </c>
       <c r="B81" s="43" t="s">
@@ -9229,7 +9233,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" ht="60">
-      <c r="A82" s="101"/>
+      <c r="A82" s="103"/>
       <c r="B82" s="43" t="s">
         <v>485</v>
       </c>
@@ -9291,7 +9295,7 @@
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="100" t="s">
+      <c r="A90" s="102" t="s">
         <v>487</v>
       </c>
       <c r="B90" s="43" t="s">
@@ -9299,7 +9303,7 @@
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="100"/>
+      <c r="A91" s="102"/>
       <c r="B91" s="43" t="s">
         <v>489</v>
       </c>
@@ -9360,10 +9364,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="97"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
@@ -9593,10 +9597,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="96" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="95"/>
+      <c r="B3" s="97"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
@@ -9658,10 +9662,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>658</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="76"/>
@@ -9679,10 +9683,10 @@
       <c r="A7" s="76"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>664</v>
       </c>
-      <c r="B8" s="95"/>
+      <c r="B8" s="97"/>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1">
       <c r="A9" s="76"/>
@@ -9709,10 +9713,10 @@
       <c r="A16" s="76"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="96" t="s">
         <v>652</v>
       </c>
-      <c r="B18" s="95"/>
+      <c r="B18" s="97"/>
     </row>
     <row r="19" spans="1:2" ht="90">
       <c r="A19" s="75" t="s">
@@ -9883,10 +9887,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="94" t="s">
+      <c r="A41" s="96" t="s">
         <v>653</v>
       </c>
-      <c r="B41" s="95"/>
+      <c r="B41" s="97"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="46" t="s">
@@ -9897,7 +9901,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="105" t="s">
+      <c r="A43" s="107" t="s">
         <v>657</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -9905,7 +9909,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="105"/>
+      <c r="A44" s="107"/>
       <c r="B44" s="19" t="s">
         <v>689</v>
       </c>
@@ -10111,7 +10115,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="120">
-      <c r="A70" s="105" t="s">
+      <c r="A70" s="107" t="s">
         <v>732</v>
       </c>
       <c r="B70" s="80" t="s">
@@ -10119,13 +10123,13 @@
       </c>
     </row>
     <row r="71" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A71" s="105"/>
+      <c r="A71" s="107"/>
       <c r="B71" s="80" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60">
-      <c r="A72" s="105" t="s">
+      <c r="A72" s="107" t="s">
         <v>740</v>
       </c>
       <c r="B72" s="80" t="s">
@@ -10133,7 +10137,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" ht="60">
-      <c r="A73" s="105"/>
+      <c r="A73" s="107"/>
       <c r="B73" s="80" t="s">
         <v>742</v>
       </c>
@@ -10259,7 +10263,7 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="105" t="s">
+      <c r="A89" s="107" t="s">
         <v>773</v>
       </c>
       <c r="B89" s="83" t="s">
@@ -10267,13 +10271,13 @@
       </c>
     </row>
     <row r="90" spans="1:2" ht="90">
-      <c r="A90" s="105"/>
+      <c r="A90" s="107"/>
       <c r="B90" s="80" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75">
-      <c r="A91" s="105"/>
+      <c r="A91" s="107"/>
       <c r="B91" s="80" t="s">
         <v>775</v>
       </c>
@@ -10428,7 +10432,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="60">
-      <c r="A111" s="105" t="s">
+      <c r="A111" s="107" t="s">
         <v>814</v>
       </c>
       <c r="B111" s="81" t="s">
@@ -10436,7 +10440,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="60">
-      <c r="A112" s="105"/>
+      <c r="A112" s="107"/>
       <c r="B112" s="81" t="s">
         <v>816</v>
       </c>
@@ -10537,10 +10541,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>643</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1">
       <c r="A3" s="6" t="s">
@@ -10563,10 +10567,10 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="96" t="s">
         <v>644</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="97"/>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1">
       <c r="A8" s="6"/>
@@ -10589,10 +10593,10 @@
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B13" s="95"/>
+      <c r="B13" s="97"/>
     </row>
     <row r="14" spans="1:2" ht="75">
       <c r="A14" s="33" t="s">
@@ -10603,7 +10607,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="120">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="106" t="s">
         <v>301</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -10611,13 +10615,13 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="240">
-      <c r="A16" s="104"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="103" t="s">
         <v>316</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -10625,19 +10629,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="120">
-      <c r="A18" s="101"/>
+      <c r="A18" s="103"/>
       <c r="B18" s="68" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135">
-      <c r="A19" s="101"/>
+      <c r="A19" s="103"/>
       <c r="B19" s="84" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="150">
-      <c r="A20" s="106" t="s">
+      <c r="A20" s="109" t="s">
         <v>430</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -10645,13 +10649,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A21" s="106"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="33" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="106" t="s">
+      <c r="A22" s="109" t="s">
         <v>408</v>
       </c>
       <c r="B22" s="33" t="s">
@@ -10659,19 +10663,19 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="60">
-      <c r="A23" s="106"/>
+      <c r="A23" s="109"/>
       <c r="B23" s="61" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="106"/>
+      <c r="A24" s="109"/>
       <c r="B24" s="33" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="109" t="s">
         <v>412</v>
       </c>
       <c r="B25" s="33" t="s">
@@ -10679,31 +10683,31 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="135">
-      <c r="A26" s="106"/>
+      <c r="A26" s="109"/>
       <c r="B26" s="33" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="106"/>
+      <c r="A27" s="109"/>
       <c r="B27" s="33" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="106"/>
+      <c r="A28" s="109"/>
       <c r="B28" s="33" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="106"/>
+      <c r="A29" s="109"/>
       <c r="B29" s="33" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="107" t="s">
+      <c r="A30" s="108" t="s">
         <v>418</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -10711,31 +10715,31 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="107"/>
+      <c r="A31" s="108"/>
       <c r="B31" s="33" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="107"/>
+      <c r="A32" s="108"/>
       <c r="B32" s="33" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="107"/>
+      <c r="A33" s="108"/>
       <c r="B33" s="33" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="107"/>
+      <c r="A34" s="108"/>
       <c r="B34" s="33" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="109" t="s">
         <v>424</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -10743,13 +10747,13 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="165">
-      <c r="A36" s="106"/>
+      <c r="A36" s="109"/>
       <c r="B36" s="33" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="106"/>
+      <c r="A37" s="109"/>
       <c r="B37" s="33" t="s">
         <v>427</v>
       </c>
@@ -10787,7 +10791,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="30">
-      <c r="A42" s="106" t="s">
+      <c r="A42" s="109" t="s">
         <v>438</v>
       </c>
       <c r="B42" s="33" t="s">
@@ -10795,7 +10799,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="75">
-      <c r="A43" s="106"/>
+      <c r="A43" s="109"/>
       <c r="B43" s="33" t="s">
         <v>440</v>
       </c>
@@ -10809,7 +10813,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="106" t="s">
+      <c r="A45" s="109" t="s">
         <v>443</v>
       </c>
       <c r="B45" s="33" t="s">
@@ -10817,7 +10821,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="106"/>
+      <c r="A46" s="109"/>
       <c r="B46" s="33" t="s">
         <v>445</v>
       </c>
@@ -10831,7 +10835,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
-      <c r="A48" s="106" t="s">
+      <c r="A48" s="109" t="s">
         <v>443</v>
       </c>
       <c r="B48" s="33" t="s">
@@ -10839,13 +10843,13 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="60">
-      <c r="A49" s="106"/>
+      <c r="A49" s="109"/>
       <c r="B49" s="33" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="107" t="s">
+      <c r="A50" s="108" t="s">
         <v>585</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10853,16 +10857,16 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="60">
-      <c r="A51" s="107"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="62" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="94" t="s">
+      <c r="A53" s="96" t="s">
         <v>833</v>
       </c>
-      <c r="B53" s="95"/>
+      <c r="B53" s="97"/>
     </row>
     <row r="54" spans="1:2" ht="45">
       <c r="A54" s="84" t="s">
@@ -10914,6 +10918,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A48:A49"/>
@@ -10923,12 +10933,6 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -10963,10 +10967,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95"/>
+      <c r="B3" s="97"/>
     </row>
     <row r="4" spans="1:2" ht="60">
       <c r="A4" s="6" t="s">
@@ -11017,7 +11021,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="106" t="s">
         <v>242</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -11025,25 +11029,25 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="104"/>
+      <c r="A11" s="106"/>
       <c r="B11" s="5" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="104"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="5" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="108"/>
+      <c r="B13" s="110"/>
     </row>
     <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="106" t="s">
         <v>247</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -11051,13 +11055,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="104"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
-      <c r="A16" s="104"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="5" t="s">
         <v>250</v>
       </c>
@@ -11087,7 +11091,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="106" t="s">
         <v>257</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -11095,7 +11099,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="104"/>
+      <c r="A21" s="106"/>
       <c r="B21" s="5" t="s">
         <v>259</v>
       </c>
@@ -11173,7 +11177,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="106" t="s">
         <v>278</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -11181,13 +11185,13 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="104"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="5" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="104"/>
+      <c r="A33" s="106"/>
       <c r="B33" s="5" t="s">
         <v>281</v>
       </c>
@@ -11241,10 +11245,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>643</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1"/>
     <row r="5" spans="1:2">
@@ -11261,13 +11265,13 @@
       <c r="A9" s="69"/>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="96" t="s">
         <v>647</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="97"/>
     </row>
     <row r="11" spans="1:2" s="19" customFormat="1">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="113" t="s">
         <v>651</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -11316,10 +11320,10 @@
       <c r="A21" s="69"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="96" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="95"/>
+      <c r="B22" s="97"/>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1">
       <c r="A23" s="69" t="s">
@@ -11370,7 +11374,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="60">
-      <c r="A29" s="107" t="s">
+      <c r="A29" s="108" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="68" t="s">
@@ -11378,13 +11382,13 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="165">
-      <c r="A30" s="107"/>
+      <c r="A30" s="108"/>
       <c r="B30" s="68" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="109" t="s">
+      <c r="A31" s="112" t="s">
         <v>624</v>
       </c>
       <c r="B31" s="68" t="s">
@@ -11392,7 +11396,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="45">
-      <c r="A32" s="109"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="68" t="s">
         <v>626</v>
       </c>
@@ -11460,7 +11464,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" s="19" customFormat="1" ht="60">
-      <c r="A41" s="105" t="s">
+      <c r="A41" s="107" t="s">
         <v>676</v>
       </c>
       <c r="B41" s="73" t="s">
@@ -11468,13 +11472,13 @@
       </c>
     </row>
     <row r="42" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A42" s="105"/>
+      <c r="A42" s="107"/>
       <c r="B42" s="73" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="105" t="s">
+      <c r="A43" s="107" t="s">
         <v>673</v>
       </c>
       <c r="B43" s="73" t="s">
@@ -11482,13 +11486,13 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="105"/>
+      <c r="A44" s="107"/>
       <c r="B44" s="73" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="75">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="107" t="s">
         <v>682</v>
       </c>
       <c r="B45" s="73" t="s">
@@ -11496,7 +11500,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="60">
-      <c r="A46" s="105"/>
+      <c r="A46" s="107"/>
       <c r="B46" s="73" t="s">
         <v>684</v>
       </c>
@@ -11519,17 +11523,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>

<commit_message>
Spring MVC + Spring Rest example
</commit_message>
<xml_diff>
--- a/Definitions/6_Definitions_Spring.xlsx
+++ b/Definitions/6_Definitions_Spring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="967" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="1017">
   <si>
     <t>Main Topic</t>
   </si>
@@ -6239,6 +6239,12 @@
   </si>
   <si>
     <t>Spring MVC Security Hello World - Java Config</t>
+  </si>
+  <si>
+    <t>Spring MVC + Rest</t>
+  </si>
+  <si>
+    <t>Cerebro -&gt; Spring -&gt; Spring MVC -&gt; Spring MVC + Spring Rest</t>
   </si>
 </sst>
 </file>
@@ -6791,10 +6797,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6802,20 +6808,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7115,7 +7121,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7486,7 +7492,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="125" t="s">
+      <c r="A12" s="127" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -7494,7 +7500,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="125"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="5" t="s">
         <v>119</v>
       </c>
@@ -7508,7 +7514,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="125" t="s">
+      <c r="A15" s="127" t="s">
         <v>122</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -7516,7 +7522,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="285">
-      <c r="A16" s="125"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="5" t="s">
         <v>124</v>
       </c>
@@ -7700,7 +7706,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="120" t="s">
+      <c r="A20" s="119" t="s">
         <v>373</v>
       </c>
       <c r="B20" s="54" t="s">
@@ -7708,7 +7714,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="120"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="29" t="s">
         <v>371</v>
       </c>
@@ -7762,7 +7768,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="120" t="s">
         <v>384</v>
       </c>
       <c r="B28" s="29" t="s">
@@ -7770,7 +7776,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="120">
-      <c r="A29" s="119"/>
+      <c r="A29" s="120"/>
       <c r="B29" s="29" t="s">
         <v>385</v>
       </c>
@@ -7872,7 +7878,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="45">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="120" t="s">
         <v>498</v>
       </c>
       <c r="B42" s="48" t="s">
@@ -7880,7 +7886,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="210">
-      <c r="A43" s="119"/>
+      <c r="A43" s="120"/>
       <c r="B43" s="48" t="s">
         <v>497</v>
       </c>
@@ -7998,7 +8004,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="45">
-      <c r="A59" s="123" t="s">
+      <c r="A59" s="124" t="s">
         <v>524</v>
       </c>
       <c r="B59" s="52" t="s">
@@ -8006,7 +8012,7 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="123"/>
+      <c r="A60" s="124"/>
       <c r="B60" s="51" t="s">
         <v>525</v>
       </c>
@@ -8100,7 +8106,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" s="19" customFormat="1" ht="75">
-      <c r="A72" s="120" t="s">
+      <c r="A72" s="119" t="s">
         <v>897</v>
       </c>
       <c r="B72" s="94" t="s">
@@ -8108,7 +8114,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" s="19" customFormat="1" ht="30">
-      <c r="A73" s="120"/>
+      <c r="A73" s="119"/>
       <c r="B73" s="94" t="s">
         <v>899</v>
       </c>
@@ -8130,7 +8136,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="60">
-      <c r="A76" s="120" t="s">
+      <c r="A76" s="119" t="s">
         <v>906</v>
       </c>
       <c r="B76" s="96" t="s">
@@ -8138,7 +8144,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="45">
-      <c r="A77" s="120"/>
+      <c r="A77" s="119"/>
       <c r="B77" s="96" t="s">
         <v>908</v>
       </c>
@@ -8193,17 +8199,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A56:A57"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A56:A57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Boot!A2" display="Up"/>
@@ -8318,7 +8324,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="180">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="119" t="s">
         <v>323</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -8326,13 +8332,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="180">
-      <c r="A15" s="120"/>
+      <c r="A15" s="119"/>
       <c r="B15" s="26" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180">
-      <c r="A16" s="120"/>
+      <c r="A16" s="119"/>
       <c r="B16" s="26" t="s">
         <v>339</v>
       </c>
@@ -8479,7 +8485,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" customHeight="1">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="124" t="s">
         <v>555</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -8487,7 +8493,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="123"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="19" t="s">
         <v>557</v>
       </c>
@@ -8689,7 +8695,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="128" t="s">
         <v>603</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -8697,7 +8703,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="126"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="66" t="s">
         <v>605</v>
       </c>
@@ -8991,7 +8997,7 @@
       <c r="B13" s="108"/>
     </row>
     <row r="14" spans="1:2" ht="75">
-      <c r="A14" s="127" t="s">
+      <c r="A14" s="125" t="s">
         <v>980</v>
       </c>
       <c r="B14" s="102" t="s">
@@ -8999,7 +9005,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="128"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="102" t="s">
         <v>982</v>
       </c>
@@ -9021,7 +9027,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
-      <c r="A18" s="128" t="s">
+      <c r="A18" s="126" t="s">
         <v>987</v>
       </c>
       <c r="B18" s="102" t="s">
@@ -9029,7 +9035,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="128"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="102" t="s">
         <v>989</v>
       </c>
@@ -11354,9 +11360,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11389,8 +11395,12 @@
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="6" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1016</v>
+      </c>
     </row>
     <row r="5" spans="1:2" s="19" customFormat="1">
       <c r="A5" s="6"/>
@@ -11475,7 +11485,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="150">
-      <c r="A20" s="120" t="s">
+      <c r="A20" s="119" t="s">
         <v>425</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -11483,13 +11493,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" ht="105">
-      <c r="A21" s="120"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="33" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="119" t="s">
         <v>403</v>
       </c>
       <c r="B22" s="33" t="s">
@@ -11497,19 +11507,19 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="60">
-      <c r="A23" s="120"/>
+      <c r="A23" s="119"/>
       <c r="B23" s="61" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="120"/>
+      <c r="A24" s="119"/>
       <c r="B24" s="33" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
-      <c r="A25" s="120" t="s">
+      <c r="A25" s="119" t="s">
         <v>407</v>
       </c>
       <c r="B25" s="33" t="s">
@@ -11517,31 +11527,31 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="135">
-      <c r="A26" s="120"/>
+      <c r="A26" s="119"/>
       <c r="B26" s="33" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="120"/>
+      <c r="A27" s="119"/>
       <c r="B27" s="33" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="120"/>
+      <c r="A28" s="119"/>
       <c r="B28" s="33" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30">
-      <c r="A29" s="120"/>
+      <c r="A29" s="119"/>
       <c r="B29" s="33" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="120" t="s">
         <v>413</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -11549,31 +11559,31 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="119"/>
+      <c r="A31" s="120"/>
       <c r="B31" s="33" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="119"/>
+      <c r="A32" s="120"/>
       <c r="B32" s="33" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="119"/>
+      <c r="A33" s="120"/>
       <c r="B33" s="33" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="119"/>
+      <c r="A34" s="120"/>
       <c r="B34" s="33" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="119" t="s">
         <v>419</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -11581,13 +11591,13 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="165">
-      <c r="A36" s="120"/>
+      <c r="A36" s="119"/>
       <c r="B36" s="33" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
-      <c r="A37" s="120"/>
+      <c r="A37" s="119"/>
       <c r="B37" s="33" t="s">
         <v>422</v>
       </c>
@@ -11625,7 +11635,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="30">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="119" t="s">
         <v>433</v>
       </c>
       <c r="B42" s="33" t="s">
@@ -11633,7 +11643,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="75">
-      <c r="A43" s="120"/>
+      <c r="A43" s="119"/>
       <c r="B43" s="33" t="s">
         <v>435</v>
       </c>
@@ -11647,7 +11657,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="120" t="s">
+      <c r="A45" s="119" t="s">
         <v>438</v>
       </c>
       <c r="B45" s="33" t="s">
@@ -11655,7 +11665,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="120"/>
+      <c r="A46" s="119"/>
       <c r="B46" s="33" t="s">
         <v>440</v>
       </c>
@@ -11669,7 +11679,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
-      <c r="A48" s="120" t="s">
+      <c r="A48" s="119" t="s">
         <v>438</v>
       </c>
       <c r="B48" s="33" t="s">
@@ -11677,13 +11687,13 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="60">
-      <c r="A49" s="120"/>
+      <c r="A49" s="119"/>
       <c r="B49" s="33" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="119" t="s">
+      <c r="A50" s="120" t="s">
         <v>580</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -11691,7 +11701,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="60">
-      <c r="A51" s="119"/>
+      <c r="A51" s="120"/>
       <c r="B51" s="62" t="s">
         <v>582</v>
       </c>
@@ -11752,12 +11762,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A48:A49"/>
@@ -11767,6 +11771,12 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A7" display="Topics"/>
@@ -12177,7 +12187,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="60">
-      <c r="A54" s="120" t="s">
+      <c r="A54" s="119" t="s">
         <v>974</v>
       </c>
       <c r="B54" s="99" t="s">
@@ -12277,9 +12287,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12319,7 +12329,7 @@
       <c r="B8" s="108"/>
     </row>
     <row r="9" spans="1:2" s="106" customFormat="1">
-      <c r="A9" s="127" t="s">
+      <c r="A9" s="125" t="s">
         <v>1014</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -12327,13 +12337,13 @@
       </c>
     </row>
     <row r="10" spans="1:2" s="106" customFormat="1">
-      <c r="A10" s="128"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="12" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="106" customFormat="1">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="124" t="s">
         <v>644</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -12341,7 +12351,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" s="106" customFormat="1">
-      <c r="A12" s="123"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="12" t="s">
         <v>637</v>
       </c>
@@ -12407,7 +12417,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="60">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="120" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="68" t="s">
@@ -12415,13 +12425,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="165">
-      <c r="A23" s="119"/>
+      <c r="A23" s="120"/>
       <c r="B23" s="68" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="123" t="s">
         <v>619</v>
       </c>
       <c r="B24" s="68" t="s">
@@ -12429,7 +12439,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="124"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="68" t="s">
         <v>621</v>
       </c>
@@ -12483,7 +12493,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="90">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="124" t="s">
         <v>665</v>
       </c>
       <c r="B32" s="73" t="s">
@@ -12491,7 +12501,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="120">
-      <c r="A33" s="123"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="73" t="s">
         <v>662</v>
       </c>
@@ -12556,6 +12566,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
@@ -12563,11 +12578,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>

</xml_diff>